<commit_message>
Nettoyage back + organisation html
Organisation du back pour spring et organisation html pour coodination
</commit_message>
<xml_diff>
--- a/So'Pain Steria.xlsx
+++ b/So'Pain Steria.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26026"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aurel\Desktop\FORMATION\Cours\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aurel\Desktop\FORMATION\Cours\Projet - So'Pain Steria\So'Pain Steria\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC7B8910-E9DA-4C58-A9F6-1D6EB0688399}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1D73A5E-F83B-4114-AAA5-FE3D1041B377}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="19440" windowHeight="10440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="243" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="245" uniqueCount="69">
   <si>
     <t>Libelle</t>
   </si>
@@ -238,6 +238,12 @@
   </si>
   <si>
     <t>Pain Campagne</t>
+  </si>
+  <si>
+    <t>Exemple insert</t>
+  </si>
+  <si>
+    <t>INSERT INTO `ingredient_line` (`ingredient_label`, `product_label`) VALUES ('Farine_T55', 'Croissant'), ('Oeuf', 'Croissant'), ('Lait', 'Croissant'), ('Sucre', 'Croissant'), ('Sel', 'Croissant'), ('Levure_boulangerie', 'Croissant'), ('Beurre', 'Croissant')</t>
   </si>
 </sst>
 </file>
@@ -261,7 +267,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -280,8 +286,20 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="15">
+  <borders count="16">
     <border>
       <left/>
       <right/>
@@ -447,11 +465,22 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="60">
+  <cellXfs count="75">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -477,22 +506,133 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -501,87 +641,36 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -600,34 +689,19 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -910,14 +984,36 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A3:V77"/>
+  <dimension ref="A1:V77"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A51" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="G53" sqref="G53"/>
+    <sheetView tabSelected="1" topLeftCell="A50" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="K68" sqref="K68"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
+    <row r="1" spans="2:21" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="2" spans="2:21" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C2" s="44" t="s">
+        <v>67</v>
+      </c>
+      <c r="D2" s="45"/>
+      <c r="E2" s="46" t="s">
+        <v>68</v>
+      </c>
+      <c r="F2" s="47"/>
+      <c r="G2" s="47"/>
+      <c r="H2" s="47"/>
+      <c r="I2" s="47"/>
+      <c r="J2" s="47"/>
+      <c r="K2" s="47"/>
+      <c r="L2" s="47"/>
+      <c r="M2" s="47"/>
+      <c r="N2" s="47"/>
+      <c r="O2" s="47"/>
+      <c r="P2" s="47"/>
+      <c r="Q2" s="48"/>
+    </row>
     <row r="3" spans="2:21" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B3" s="3"/>
       <c r="C3" s="3"/>
@@ -927,32 +1023,21 @@
       <c r="G3" s="3"/>
       <c r="H3" s="3"/>
       <c r="I3" s="3"/>
-      <c r="J3" s="3"/>
-      <c r="K3" s="3"/>
-      <c r="L3" s="3"/>
-      <c r="M3" s="3"/>
-      <c r="N3" s="3"/>
-      <c r="O3" s="3"/>
-      <c r="P3" s="3"/>
-      <c r="Q3" s="3"/>
-      <c r="R3" s="3"/>
-      <c r="S3" s="3"/>
-      <c r="T3" s="3"/>
       <c r="U3" s="3"/>
     </row>
     <row r="4" spans="2:21" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B4" s="9" t="s">
+      <c r="B4" s="15" t="s">
         <v>0</v>
       </c>
-      <c r="C4" s="10"/>
-      <c r="D4" s="9" t="s">
-        <v>1</v>
-      </c>
-      <c r="E4" s="19"/>
+      <c r="C4" s="16"/>
+      <c r="D4" s="15" t="s">
+        <v>1</v>
+      </c>
+      <c r="E4" s="17"/>
       <c r="F4" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="G4" s="59"/>
+      <c r="G4" s="2"/>
       <c r="H4" s="3"/>
       <c r="I4" s="3"/>
       <c r="J4" s="3"/>
@@ -969,15 +1054,15 @@
       <c r="U4" s="3"/>
     </row>
     <row r="5" spans="2:21" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B5" s="9" t="s">
+      <c r="B5" s="22" t="s">
         <v>18</v>
       </c>
-      <c r="C5" s="10"/>
-      <c r="D5" s="28" t="s">
+      <c r="C5" s="23"/>
+      <c r="D5" s="18" t="s">
         <v>4</v>
       </c>
-      <c r="E5" s="29"/>
-      <c r="F5" s="50">
+      <c r="E5" s="19"/>
+      <c r="F5" s="9">
         <v>1</v>
       </c>
       <c r="G5" s="4">
@@ -985,15 +1070,15 @@
         <v>4</v>
       </c>
       <c r="H5" s="3"/>
-      <c r="I5" s="9" t="s">
+      <c r="I5" s="22" t="s">
         <v>20</v>
       </c>
-      <c r="J5" s="19"/>
-      <c r="K5" s="28" t="s">
+      <c r="J5" s="49"/>
+      <c r="K5" s="18" t="s">
         <v>4</v>
       </c>
-      <c r="L5" s="29"/>
-      <c r="M5" s="50">
+      <c r="L5" s="19"/>
+      <c r="M5" s="9">
         <v>1</v>
       </c>
       <c r="N5" s="4">
@@ -1001,15 +1086,15 @@
         <v>4</v>
       </c>
       <c r="O5" s="3"/>
-      <c r="P5" s="9" t="s">
+      <c r="P5" s="22" t="s">
         <v>39</v>
       </c>
-      <c r="Q5" s="19"/>
-      <c r="R5" s="28" t="s">
+      <c r="Q5" s="49"/>
+      <c r="R5" s="18" t="s">
         <v>4</v>
       </c>
-      <c r="S5" s="29"/>
-      <c r="T5" s="50">
+      <c r="S5" s="19"/>
+      <c r="T5" s="9">
         <v>1</v>
       </c>
       <c r="U5" s="4">
@@ -1018,187 +1103,187 @@
       </c>
     </row>
     <row r="6" spans="2:21" x14ac:dyDescent="0.3">
-      <c r="B6" s="11"/>
-      <c r="C6" s="12"/>
-      <c r="D6" s="26" t="s">
+      <c r="B6" s="24"/>
+      <c r="C6" s="25"/>
+      <c r="D6" s="20" t="s">
         <v>6</v>
       </c>
-      <c r="E6" s="27"/>
-      <c r="F6" s="51">
-        <v>1</v>
-      </c>
-      <c r="G6" s="58"/>
+      <c r="E6" s="21"/>
+      <c r="F6" s="10">
+        <v>1</v>
+      </c>
+      <c r="G6" s="3"/>
       <c r="H6" s="3"/>
-      <c r="I6" s="11"/>
-      <c r="J6" s="20"/>
-      <c r="K6" s="26" t="s">
+      <c r="I6" s="24"/>
+      <c r="J6" s="50"/>
+      <c r="K6" s="20" t="s">
         <v>6</v>
       </c>
-      <c r="L6" s="27"/>
-      <c r="M6" s="51">
-        <v>1</v>
-      </c>
-      <c r="N6" s="58"/>
+      <c r="L6" s="21"/>
+      <c r="M6" s="10">
+        <v>1</v>
+      </c>
+      <c r="N6" s="3"/>
       <c r="O6" s="3"/>
-      <c r="P6" s="11"/>
-      <c r="Q6" s="20"/>
-      <c r="R6" s="26" t="s">
+      <c r="P6" s="24"/>
+      <c r="Q6" s="50"/>
+      <c r="R6" s="20" t="s">
         <v>6</v>
       </c>
-      <c r="S6" s="27"/>
-      <c r="T6" s="51">
+      <c r="S6" s="21"/>
+      <c r="T6" s="10">
         <v>1</v>
       </c>
       <c r="U6" s="3"/>
     </row>
     <row r="7" spans="2:21" x14ac:dyDescent="0.3">
-      <c r="B7" s="11"/>
-      <c r="C7" s="12"/>
-      <c r="D7" s="26" t="s">
+      <c r="B7" s="24"/>
+      <c r="C7" s="25"/>
+      <c r="D7" s="20" t="s">
         <v>7</v>
       </c>
-      <c r="E7" s="27"/>
-      <c r="F7" s="51">
-        <v>1</v>
-      </c>
-      <c r="G7" s="58"/>
+      <c r="E7" s="21"/>
+      <c r="F7" s="10">
+        <v>1</v>
+      </c>
+      <c r="G7" s="3"/>
       <c r="H7" s="3"/>
-      <c r="I7" s="11"/>
-      <c r="J7" s="20"/>
-      <c r="K7" s="26" t="s">
+      <c r="I7" s="24"/>
+      <c r="J7" s="50"/>
+      <c r="K7" s="20" t="s">
         <v>7</v>
       </c>
-      <c r="L7" s="27"/>
-      <c r="M7" s="51">
-        <v>1</v>
-      </c>
-      <c r="N7" s="58"/>
+      <c r="L7" s="21"/>
+      <c r="M7" s="10">
+        <v>1</v>
+      </c>
+      <c r="N7" s="3"/>
       <c r="O7" s="3"/>
-      <c r="P7" s="11"/>
-      <c r="Q7" s="20"/>
-      <c r="R7" s="26" t="s">
+      <c r="P7" s="24"/>
+      <c r="Q7" s="50"/>
+      <c r="R7" s="20" t="s">
         <v>7</v>
       </c>
-      <c r="S7" s="27"/>
-      <c r="T7" s="51">
+      <c r="S7" s="21"/>
+      <c r="T7" s="10">
         <v>1</v>
       </c>
       <c r="U7" s="3"/>
     </row>
     <row r="8" spans="2:21" x14ac:dyDescent="0.3">
-      <c r="B8" s="11"/>
-      <c r="C8" s="12"/>
-      <c r="D8" s="26" t="s">
+      <c r="B8" s="24"/>
+      <c r="C8" s="25"/>
+      <c r="D8" s="20" t="s">
         <v>8</v>
       </c>
-      <c r="E8" s="27"/>
-      <c r="F8" s="51"/>
-      <c r="G8" s="58"/>
+      <c r="E8" s="21"/>
+      <c r="F8" s="10"/>
+      <c r="G8" s="3"/>
       <c r="H8" s="3"/>
-      <c r="I8" s="11"/>
-      <c r="J8" s="20"/>
-      <c r="K8" s="26" t="s">
+      <c r="I8" s="24"/>
+      <c r="J8" s="50"/>
+      <c r="K8" s="20" t="s">
         <v>8</v>
       </c>
-      <c r="L8" s="27"/>
-      <c r="M8" s="51"/>
-      <c r="N8" s="58"/>
+      <c r="L8" s="21"/>
+      <c r="M8" s="10"/>
+      <c r="N8" s="3"/>
       <c r="O8" s="3"/>
-      <c r="P8" s="11"/>
-      <c r="Q8" s="20"/>
-      <c r="R8" s="26" t="s">
+      <c r="P8" s="24"/>
+      <c r="Q8" s="50"/>
+      <c r="R8" s="20" t="s">
         <v>8</v>
       </c>
-      <c r="S8" s="27"/>
-      <c r="T8" s="51"/>
+      <c r="S8" s="21"/>
+      <c r="T8" s="10"/>
       <c r="U8" s="3"/>
     </row>
     <row r="9" spans="2:21" x14ac:dyDescent="0.3">
-      <c r="B9" s="11"/>
-      <c r="C9" s="12"/>
-      <c r="D9" s="26" t="s">
+      <c r="B9" s="24"/>
+      <c r="C9" s="25"/>
+      <c r="D9" s="20" t="s">
         <v>15</v>
       </c>
-      <c r="E9" s="27"/>
-      <c r="F9" s="51"/>
-      <c r="G9" s="58"/>
+      <c r="E9" s="21"/>
+      <c r="F9" s="10"/>
+      <c r="G9" s="3"/>
       <c r="H9" s="3"/>
-      <c r="I9" s="11"/>
-      <c r="J9" s="20"/>
-      <c r="K9" s="26" t="s">
+      <c r="I9" s="24"/>
+      <c r="J9" s="50"/>
+      <c r="K9" s="20" t="s">
         <v>15</v>
       </c>
-      <c r="L9" s="27"/>
-      <c r="M9" s="51"/>
-      <c r="N9" s="58"/>
+      <c r="L9" s="21"/>
+      <c r="M9" s="10"/>
+      <c r="N9" s="3"/>
       <c r="O9" s="3"/>
-      <c r="P9" s="11"/>
-      <c r="Q9" s="20"/>
-      <c r="R9" s="26" t="s">
+      <c r="P9" s="24"/>
+      <c r="Q9" s="50"/>
+      <c r="R9" s="20" t="s">
         <v>15</v>
       </c>
-      <c r="S9" s="27"/>
-      <c r="T9" s="51"/>
+      <c r="S9" s="21"/>
+      <c r="T9" s="10"/>
       <c r="U9" s="3"/>
     </row>
     <row r="10" spans="2:21" x14ac:dyDescent="0.3">
-      <c r="B10" s="11"/>
-      <c r="C10" s="12"/>
-      <c r="D10" s="26" t="s">
+      <c r="B10" s="24"/>
+      <c r="C10" s="25"/>
+      <c r="D10" s="20" t="s">
         <v>9</v>
       </c>
-      <c r="E10" s="27"/>
-      <c r="F10" s="51"/>
-      <c r="G10" s="58"/>
+      <c r="E10" s="21"/>
+      <c r="F10" s="10"/>
+      <c r="G10" s="3"/>
       <c r="H10" s="3"/>
-      <c r="I10" s="11"/>
-      <c r="J10" s="20"/>
-      <c r="K10" s="26" t="s">
+      <c r="I10" s="24"/>
+      <c r="J10" s="50"/>
+      <c r="K10" s="20" t="s">
         <v>9</v>
       </c>
-      <c r="L10" s="27"/>
-      <c r="M10" s="51"/>
-      <c r="N10" s="58"/>
+      <c r="L10" s="21"/>
+      <c r="M10" s="10"/>
+      <c r="N10" s="3"/>
       <c r="O10" s="3"/>
-      <c r="P10" s="11"/>
-      <c r="Q10" s="20"/>
-      <c r="R10" s="26" t="s">
+      <c r="P10" s="24"/>
+      <c r="Q10" s="50"/>
+      <c r="R10" s="20" t="s">
         <v>9</v>
       </c>
-      <c r="S10" s="27"/>
-      <c r="T10" s="51"/>
+      <c r="S10" s="21"/>
+      <c r="T10" s="10"/>
       <c r="U10" s="3"/>
     </row>
     <row r="11" spans="2:21" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B11" s="13"/>
-      <c r="C11" s="14"/>
-      <c r="D11" s="56" t="s">
+      <c r="B11" s="26"/>
+      <c r="C11" s="27"/>
+      <c r="D11" s="28" t="s">
         <v>10</v>
       </c>
-      <c r="E11" s="57"/>
-      <c r="F11" s="52">
-        <v>1</v>
-      </c>
-      <c r="G11" s="58"/>
+      <c r="E11" s="29"/>
+      <c r="F11" s="11">
+        <v>1</v>
+      </c>
+      <c r="G11" s="3"/>
       <c r="H11" s="3"/>
-      <c r="I11" s="11"/>
-      <c r="J11" s="20"/>
-      <c r="K11" s="26" t="s">
+      <c r="I11" s="24"/>
+      <c r="J11" s="50"/>
+      <c r="K11" s="20" t="s">
         <v>10</v>
       </c>
-      <c r="L11" s="27"/>
-      <c r="M11" s="51">
-        <v>1</v>
-      </c>
-      <c r="N11" s="58"/>
+      <c r="L11" s="21"/>
+      <c r="M11" s="10">
+        <v>1</v>
+      </c>
+      <c r="N11" s="3"/>
       <c r="O11" s="3"/>
-      <c r="P11" s="11"/>
-      <c r="Q11" s="20"/>
-      <c r="R11" s="26" t="s">
+      <c r="P11" s="24"/>
+      <c r="Q11" s="50"/>
+      <c r="R11" s="20" t="s">
         <v>10</v>
       </c>
-      <c r="S11" s="27"/>
-      <c r="T11" s="51">
+      <c r="S11" s="21"/>
+      <c r="T11" s="10">
         <v>1</v>
       </c>
       <c r="U11" s="3"/>
@@ -1211,22 +1296,22 @@
       <c r="F12" s="3"/>
       <c r="G12" s="3"/>
       <c r="H12" s="3"/>
-      <c r="I12" s="13"/>
-      <c r="J12" s="21"/>
-      <c r="K12" s="56" t="s">
+      <c r="I12" s="26"/>
+      <c r="J12" s="51"/>
+      <c r="K12" s="28" t="s">
         <v>11</v>
       </c>
-      <c r="L12" s="57"/>
-      <c r="M12" s="52"/>
-      <c r="N12" s="58"/>
+      <c r="L12" s="29"/>
+      <c r="M12" s="11"/>
+      <c r="N12" s="3"/>
       <c r="O12" s="3"/>
-      <c r="P12" s="11"/>
-      <c r="Q12" s="20"/>
-      <c r="R12" s="26" t="s">
+      <c r="P12" s="24"/>
+      <c r="Q12" s="50"/>
+      <c r="R12" s="20" t="s">
         <v>16</v>
       </c>
-      <c r="S12" s="27"/>
-      <c r="T12" s="51"/>
+      <c r="S12" s="21"/>
+      <c r="T12" s="10"/>
       <c r="U12" s="3"/>
     </row>
     <row r="13" spans="2:21" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -1244,13 +1329,13 @@
       <c r="M13" s="3"/>
       <c r="N13" s="3"/>
       <c r="O13" s="3"/>
-      <c r="P13" s="13"/>
-      <c r="Q13" s="21"/>
-      <c r="R13" s="17" t="s">
+      <c r="P13" s="26"/>
+      <c r="Q13" s="51"/>
+      <c r="R13" s="39" t="s">
         <v>41</v>
       </c>
-      <c r="S13" s="18"/>
-      <c r="T13" s="52">
+      <c r="S13" s="40"/>
+      <c r="T13" s="11">
         <f>3-3</f>
         <v>0</v>
       </c>
@@ -1301,29 +1386,29 @@
       <c r="U15" s="3"/>
     </row>
     <row r="16" spans="2:21" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B16" s="9" t="s">
+      <c r="B16" s="22" t="s">
         <v>21</v>
       </c>
-      <c r="C16" s="10"/>
-      <c r="D16" s="28" t="s">
+      <c r="C16" s="23"/>
+      <c r="D16" s="18" t="s">
         <v>42</v>
       </c>
-      <c r="E16" s="29"/>
-      <c r="F16" s="50"/>
+      <c r="E16" s="19"/>
+      <c r="F16" s="9"/>
       <c r="G16" s="4">
         <f>SUM(F16:F22)</f>
         <v>3</v>
       </c>
       <c r="H16" s="3"/>
-      <c r="I16" s="9" t="s">
+      <c r="I16" s="22" t="s">
         <v>22</v>
       </c>
-      <c r="J16" s="10"/>
-      <c r="K16" s="28" t="s">
+      <c r="J16" s="23"/>
+      <c r="K16" s="18" t="s">
         <v>4</v>
       </c>
-      <c r="L16" s="29"/>
-      <c r="M16" s="50">
+      <c r="L16" s="19"/>
+      <c r="M16" s="9">
         <v>1</v>
       </c>
       <c r="N16" s="4">
@@ -1331,15 +1416,15 @@
         <v>4</v>
       </c>
       <c r="O16" s="3"/>
-      <c r="P16" s="9" t="s">
+      <c r="P16" s="22" t="s">
         <v>23</v>
       </c>
-      <c r="Q16" s="19"/>
-      <c r="R16" s="28" t="s">
+      <c r="Q16" s="49"/>
+      <c r="R16" s="18" t="s">
         <v>4</v>
       </c>
-      <c r="S16" s="29"/>
-      <c r="T16" s="50">
+      <c r="S16" s="19"/>
+      <c r="T16" s="9">
         <v>1</v>
       </c>
       <c r="U16" s="4">
@@ -1348,188 +1433,188 @@
       </c>
     </row>
     <row r="17" spans="2:22" x14ac:dyDescent="0.3">
-      <c r="B17" s="11"/>
-      <c r="C17" s="12"/>
-      <c r="D17" s="26" t="s">
+      <c r="B17" s="24"/>
+      <c r="C17" s="25"/>
+      <c r="D17" s="20" t="s">
         <v>10</v>
       </c>
-      <c r="E17" s="27"/>
-      <c r="F17" s="51">
-        <v>1</v>
-      </c>
-      <c r="G17" s="58"/>
+      <c r="E17" s="21"/>
+      <c r="F17" s="10">
+        <v>1</v>
+      </c>
+      <c r="G17" s="3"/>
       <c r="H17" s="3"/>
-      <c r="I17" s="11"/>
-      <c r="J17" s="12"/>
-      <c r="K17" s="26" t="s">
+      <c r="I17" s="24"/>
+      <c r="J17" s="25"/>
+      <c r="K17" s="20" t="s">
         <v>6</v>
       </c>
-      <c r="L17" s="27"/>
-      <c r="M17" s="51">
-        <v>1</v>
-      </c>
-      <c r="N17" s="58"/>
+      <c r="L17" s="21"/>
+      <c r="M17" s="10">
+        <v>1</v>
+      </c>
+      <c r="N17" s="3"/>
       <c r="O17" s="3"/>
-      <c r="P17" s="11"/>
-      <c r="Q17" s="20"/>
-      <c r="R17" s="26" t="s">
+      <c r="P17" s="24"/>
+      <c r="Q17" s="50"/>
+      <c r="R17" s="20" t="s">
         <v>6</v>
       </c>
-      <c r="S17" s="27"/>
-      <c r="T17" s="51">
+      <c r="S17" s="21"/>
+      <c r="T17" s="10">
         <v>1</v>
       </c>
       <c r="U17" s="3"/>
     </row>
     <row r="18" spans="2:22" x14ac:dyDescent="0.3">
-      <c r="B18" s="11"/>
-      <c r="C18" s="12"/>
-      <c r="D18" s="26" t="s">
+      <c r="B18" s="24"/>
+      <c r="C18" s="25"/>
+      <c r="D18" s="20" t="s">
         <v>6</v>
       </c>
-      <c r="E18" s="27"/>
-      <c r="F18" s="51">
-        <v>1</v>
-      </c>
-      <c r="G18" s="58"/>
+      <c r="E18" s="21"/>
+      <c r="F18" s="10">
+        <v>1</v>
+      </c>
+      <c r="G18" s="3"/>
       <c r="H18" s="3"/>
-      <c r="I18" s="11"/>
-      <c r="J18" s="12"/>
-      <c r="K18" s="26" t="s">
+      <c r="I18" s="24"/>
+      <c r="J18" s="25"/>
+      <c r="K18" s="20" t="s">
         <v>7</v>
       </c>
-      <c r="L18" s="27"/>
-      <c r="M18" s="51">
-        <v>1</v>
-      </c>
-      <c r="N18" s="58"/>
+      <c r="L18" s="21"/>
+      <c r="M18" s="10">
+        <v>1</v>
+      </c>
+      <c r="N18" s="3"/>
       <c r="O18" s="3"/>
-      <c r="P18" s="11"/>
-      <c r="Q18" s="20"/>
-      <c r="R18" s="26" t="s">
+      <c r="P18" s="24"/>
+      <c r="Q18" s="50"/>
+      <c r="R18" s="20" t="s">
         <v>7</v>
       </c>
-      <c r="S18" s="27"/>
-      <c r="T18" s="51">
+      <c r="S18" s="21"/>
+      <c r="T18" s="10">
         <v>1</v>
       </c>
       <c r="U18" s="3"/>
     </row>
     <row r="19" spans="2:22" x14ac:dyDescent="0.3">
-      <c r="B19" s="11"/>
-      <c r="C19" s="12"/>
-      <c r="D19" s="26" t="s">
+      <c r="B19" s="24"/>
+      <c r="C19" s="25"/>
+      <c r="D19" s="20" t="s">
         <v>17</v>
       </c>
-      <c r="E19" s="27"/>
-      <c r="F19" s="51"/>
-      <c r="G19" s="58"/>
+      <c r="E19" s="21"/>
+      <c r="F19" s="10"/>
+      <c r="G19" s="3"/>
       <c r="H19" s="3"/>
-      <c r="I19" s="11"/>
-      <c r="J19" s="12"/>
-      <c r="K19" s="26" t="s">
+      <c r="I19" s="24"/>
+      <c r="J19" s="25"/>
+      <c r="K19" s="20" t="s">
         <v>8</v>
       </c>
-      <c r="L19" s="27"/>
-      <c r="M19" s="51"/>
-      <c r="N19" s="58"/>
+      <c r="L19" s="21"/>
+      <c r="M19" s="10"/>
+      <c r="N19" s="3"/>
       <c r="O19" s="3"/>
-      <c r="P19" s="11"/>
-      <c r="Q19" s="20"/>
-      <c r="R19" s="26" t="s">
+      <c r="P19" s="24"/>
+      <c r="Q19" s="50"/>
+      <c r="R19" s="20" t="s">
         <v>8</v>
       </c>
-      <c r="S19" s="27"/>
-      <c r="T19" s="51"/>
+      <c r="S19" s="21"/>
+      <c r="T19" s="10"/>
       <c r="U19" s="3"/>
     </row>
     <row r="20" spans="2:22" x14ac:dyDescent="0.3">
-      <c r="B20" s="11"/>
-      <c r="C20" s="12"/>
-      <c r="D20" s="26" t="s">
+      <c r="B20" s="24"/>
+      <c r="C20" s="25"/>
+      <c r="D20" s="20" t="s">
         <v>8</v>
       </c>
-      <c r="E20" s="27"/>
-      <c r="F20" s="51"/>
-      <c r="G20" s="58"/>
+      <c r="E20" s="21"/>
+      <c r="F20" s="10"/>
+      <c r="G20" s="3"/>
       <c r="H20" s="3"/>
-      <c r="I20" s="11"/>
-      <c r="J20" s="12"/>
-      <c r="K20" s="26" t="s">
+      <c r="I20" s="24"/>
+      <c r="J20" s="25"/>
+      <c r="K20" s="20" t="s">
         <v>15</v>
       </c>
-      <c r="L20" s="27"/>
-      <c r="M20" s="51"/>
-      <c r="N20" s="58"/>
+      <c r="L20" s="21"/>
+      <c r="M20" s="10"/>
+      <c r="N20" s="3"/>
       <c r="O20" s="3"/>
-      <c r="P20" s="11"/>
-      <c r="Q20" s="20"/>
-      <c r="R20" s="26" t="s">
+      <c r="P20" s="24"/>
+      <c r="Q20" s="50"/>
+      <c r="R20" s="20" t="s">
         <v>15</v>
       </c>
-      <c r="S20" s="27"/>
-      <c r="T20" s="51"/>
+      <c r="S20" s="21"/>
+      <c r="T20" s="10"/>
       <c r="U20" s="3"/>
     </row>
     <row r="21" spans="2:22" x14ac:dyDescent="0.3">
-      <c r="B21" s="11"/>
-      <c r="C21" s="12"/>
-      <c r="D21" s="26" t="s">
+      <c r="B21" s="24"/>
+      <c r="C21" s="25"/>
+      <c r="D21" s="20" t="s">
         <v>43</v>
       </c>
-      <c r="E21" s="27"/>
-      <c r="F21" s="51"/>
-      <c r="G21" s="58"/>
+      <c r="E21" s="21"/>
+      <c r="F21" s="10"/>
+      <c r="G21" s="3"/>
       <c r="H21" s="3"/>
-      <c r="I21" s="11"/>
-      <c r="J21" s="12"/>
-      <c r="K21" s="26" t="s">
+      <c r="I21" s="24"/>
+      <c r="J21" s="25"/>
+      <c r="K21" s="20" t="s">
         <v>9</v>
       </c>
-      <c r="L21" s="27"/>
-      <c r="M21" s="51"/>
-      <c r="N21" s="58"/>
+      <c r="L21" s="21"/>
+      <c r="M21" s="10"/>
+      <c r="N21" s="3"/>
       <c r="O21" s="3"/>
-      <c r="P21" s="11"/>
-      <c r="Q21" s="20"/>
-      <c r="R21" s="26" t="s">
+      <c r="P21" s="24"/>
+      <c r="Q21" s="50"/>
+      <c r="R21" s="20" t="s">
         <v>9</v>
       </c>
-      <c r="S21" s="27"/>
-      <c r="T21" s="51"/>
+      <c r="S21" s="21"/>
+      <c r="T21" s="10"/>
       <c r="U21" s="3"/>
     </row>
     <row r="22" spans="2:22" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B22" s="13"/>
-      <c r="C22" s="14"/>
-      <c r="D22" s="17" t="s">
+      <c r="B22" s="26"/>
+      <c r="C22" s="27"/>
+      <c r="D22" s="39" t="s">
         <v>44</v>
       </c>
-      <c r="E22" s="18"/>
-      <c r="F22" s="52">
+      <c r="E22" s="40"/>
+      <c r="F22" s="11">
         <f>2-1</f>
         <v>1</v>
       </c>
-      <c r="G22" s="58"/>
+      <c r="G22" s="3"/>
       <c r="H22" s="3"/>
-      <c r="I22" s="11"/>
-      <c r="J22" s="12"/>
-      <c r="K22" s="26" t="s">
+      <c r="I22" s="24"/>
+      <c r="J22" s="25"/>
+      <c r="K22" s="20" t="s">
         <v>10</v>
       </c>
-      <c r="L22" s="27"/>
-      <c r="M22" s="51">
-        <v>1</v>
-      </c>
-      <c r="N22" s="58"/>
+      <c r="L22" s="21"/>
+      <c r="M22" s="10">
+        <v>1</v>
+      </c>
+      <c r="N22" s="3"/>
       <c r="O22" s="3"/>
-      <c r="P22" s="11"/>
-      <c r="Q22" s="20"/>
-      <c r="R22" s="26" t="s">
+      <c r="P22" s="24"/>
+      <c r="Q22" s="50"/>
+      <c r="R22" s="20" t="s">
         <v>10</v>
       </c>
-      <c r="S22" s="27"/>
-      <c r="T22" s="51">
+      <c r="S22" s="21"/>
+      <c r="T22" s="10">
         <v>1</v>
       </c>
       <c r="U22" s="3"/>
@@ -1542,25 +1627,25 @@
       <c r="F23" s="3"/>
       <c r="G23" s="3"/>
       <c r="H23" s="3"/>
-      <c r="I23" s="13"/>
-      <c r="J23" s="14"/>
-      <c r="K23" s="17" t="s">
+      <c r="I23" s="26"/>
+      <c r="J23" s="27"/>
+      <c r="K23" s="39" t="s">
         <v>41</v>
       </c>
-      <c r="L23" s="18"/>
-      <c r="M23" s="52">
+      <c r="L23" s="40"/>
+      <c r="M23" s="11">
         <f>3-3</f>
         <v>0</v>
       </c>
-      <c r="N23" s="58"/>
+      <c r="N23" s="3"/>
       <c r="O23" s="3"/>
-      <c r="P23" s="13"/>
-      <c r="Q23" s="21"/>
-      <c r="R23" s="17" t="s">
+      <c r="P23" s="26"/>
+      <c r="Q23" s="51"/>
+      <c r="R23" s="39" t="s">
         <v>41</v>
       </c>
-      <c r="S23" s="18"/>
-      <c r="T23" s="52">
+      <c r="S23" s="40"/>
+      <c r="T23" s="11">
         <f>3-3</f>
         <v>0</v>
       </c>
@@ -1612,15 +1697,15 @@
       <c r="V25" s="1"/>
     </row>
     <row r="26" spans="2:22" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B26" s="9" t="s">
+      <c r="B26" s="30" t="s">
         <v>24</v>
       </c>
-      <c r="C26" s="10"/>
-      <c r="D26" s="28" t="s">
+      <c r="C26" s="31"/>
+      <c r="D26" s="18" t="s">
         <v>5</v>
       </c>
-      <c r="E26" s="29"/>
-      <c r="F26" s="50">
+      <c r="E26" s="19"/>
+      <c r="F26" s="9">
         <v>1</v>
       </c>
       <c r="G26" s="4">
@@ -1628,15 +1713,15 @@
         <v>4</v>
       </c>
       <c r="H26" s="3"/>
-      <c r="I26" s="9" t="s">
+      <c r="I26" s="30" t="s">
         <v>25</v>
       </c>
-      <c r="J26" s="10"/>
-      <c r="K26" s="28" t="s">
+      <c r="J26" s="31"/>
+      <c r="K26" s="18" t="s">
         <v>4</v>
       </c>
-      <c r="L26" s="29"/>
-      <c r="M26" s="50">
+      <c r="L26" s="19"/>
+      <c r="M26" s="9">
         <v>1</v>
       </c>
       <c r="N26" s="4">
@@ -1644,15 +1729,15 @@
         <v>1</v>
       </c>
       <c r="O26" s="3"/>
-      <c r="P26" s="9" t="s">
+      <c r="P26" s="30" t="s">
         <v>66</v>
       </c>
-      <c r="Q26" s="10"/>
-      <c r="R26" s="28" t="s">
+      <c r="Q26" s="31"/>
+      <c r="R26" s="18" t="s">
         <v>4</v>
       </c>
-      <c r="S26" s="29"/>
-      <c r="T26" s="50">
+      <c r="S26" s="19"/>
+      <c r="T26" s="9">
         <v>1</v>
       </c>
       <c r="U26" s="4">
@@ -1662,98 +1747,98 @@
       <c r="V26" s="1"/>
     </row>
     <row r="27" spans="2:22" x14ac:dyDescent="0.3">
-      <c r="B27" s="11"/>
-      <c r="C27" s="12"/>
-      <c r="D27" s="26" t="s">
+      <c r="B27" s="32"/>
+      <c r="C27" s="33"/>
+      <c r="D27" s="20" t="s">
         <v>6</v>
       </c>
-      <c r="E27" s="27"/>
-      <c r="F27" s="51">
-        <v>1</v>
-      </c>
-      <c r="G27" s="58"/>
+      <c r="E27" s="21"/>
+      <c r="F27" s="10">
+        <v>1</v>
+      </c>
+      <c r="G27" s="3"/>
       <c r="H27" s="3"/>
-      <c r="I27" s="11"/>
-      <c r="J27" s="12"/>
-      <c r="K27" s="26" t="s">
+      <c r="I27" s="32"/>
+      <c r="J27" s="33"/>
+      <c r="K27" s="20" t="s">
         <v>9</v>
       </c>
-      <c r="L27" s="27"/>
-      <c r="M27" s="51"/>
-      <c r="N27" s="58"/>
+      <c r="L27" s="21"/>
+      <c r="M27" s="10"/>
+      <c r="N27" s="3"/>
       <c r="O27" s="3"/>
-      <c r="P27" s="11"/>
-      <c r="Q27" s="12"/>
-      <c r="R27" s="26" t="s">
+      <c r="P27" s="32"/>
+      <c r="Q27" s="33"/>
+      <c r="R27" s="20" t="s">
         <v>9</v>
       </c>
-      <c r="S27" s="27"/>
-      <c r="T27" s="51"/>
+      <c r="S27" s="21"/>
+      <c r="T27" s="10"/>
       <c r="U27" s="3"/>
     </row>
     <row r="28" spans="2:22" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B28" s="11"/>
-      <c r="C28" s="12"/>
-      <c r="D28" s="26" t="s">
+      <c r="B28" s="32"/>
+      <c r="C28" s="33"/>
+      <c r="D28" s="20" t="s">
         <v>7</v>
       </c>
-      <c r="E28" s="27"/>
-      <c r="F28" s="51">
-        <v>1</v>
-      </c>
-      <c r="G28" s="58"/>
+      <c r="E28" s="21"/>
+      <c r="F28" s="10">
+        <v>1</v>
+      </c>
+      <c r="G28" s="3"/>
       <c r="H28" s="3"/>
-      <c r="I28" s="13"/>
-      <c r="J28" s="14"/>
-      <c r="K28" s="56" t="s">
+      <c r="I28" s="34"/>
+      <c r="J28" s="35"/>
+      <c r="K28" s="28" t="s">
         <v>15</v>
       </c>
-      <c r="L28" s="57"/>
-      <c r="M28" s="52"/>
-      <c r="N28" s="58"/>
+      <c r="L28" s="29"/>
+      <c r="M28" s="11"/>
+      <c r="N28" s="3"/>
       <c r="O28" s="3"/>
-      <c r="P28" s="13"/>
-      <c r="Q28" s="14"/>
-      <c r="R28" s="56" t="s">
+      <c r="P28" s="34"/>
+      <c r="Q28" s="35"/>
+      <c r="R28" s="28" t="s">
         <v>15</v>
       </c>
-      <c r="S28" s="57"/>
-      <c r="T28" s="52"/>
+      <c r="S28" s="29"/>
+      <c r="T28" s="11"/>
       <c r="U28" s="3"/>
     </row>
     <row r="29" spans="2:22" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B29" s="11"/>
-      <c r="C29" s="12"/>
-      <c r="D29" s="26" t="s">
+      <c r="B29" s="32"/>
+      <c r="C29" s="33"/>
+      <c r="D29" s="20" t="s">
         <v>8</v>
       </c>
-      <c r="E29" s="27"/>
-      <c r="F29" s="51"/>
-      <c r="G29" s="58"/>
+      <c r="E29" s="21"/>
+      <c r="F29" s="10"/>
+      <c r="G29" s="3"/>
       <c r="H29" s="3"/>
       <c r="I29" s="2"/>
       <c r="J29" s="2"/>
-      <c r="K29" s="32"/>
-      <c r="L29" s="32"/>
+      <c r="K29" s="41"/>
+      <c r="L29" s="41"/>
       <c r="M29" s="3"/>
       <c r="N29" s="3"/>
       <c r="O29" s="3"/>
       <c r="P29" s="2"/>
       <c r="Q29" s="2"/>
-      <c r="R29" s="32"/>
-      <c r="S29" s="32"/>
+      <c r="R29" s="41"/>
+      <c r="S29" s="41"/>
       <c r="T29" s="3"/>
       <c r="U29" s="3"/>
     </row>
     <row r="30" spans="2:22" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B30" s="11"/>
-      <c r="C30" s="12"/>
-      <c r="D30" s="26" t="s">
+      <c r="B30" s="32"/>
+      <c r="C30" s="33"/>
+      <c r="D30" s="20" t="s">
         <v>15</v>
       </c>
-      <c r="E30" s="27"/>
-      <c r="F30" s="51"/>
-      <c r="G30" s="58"/>
+      <c r="E30" s="21"/>
+      <c r="F30" s="10"/>
+      <c r="G30" s="3"/>
       <c r="H30" s="3"/>
       <c r="I30" s="3"/>
       <c r="J30" s="3"/>
@@ -1762,15 +1847,15 @@
       <c r="M30" s="3"/>
       <c r="N30" s="3"/>
       <c r="O30" s="3"/>
-      <c r="P30" s="9" t="s">
+      <c r="P30" s="30" t="s">
         <v>27</v>
       </c>
-      <c r="Q30" s="10"/>
-      <c r="R30" s="28" t="s">
+      <c r="Q30" s="31"/>
+      <c r="R30" s="18" t="s">
         <v>4</v>
       </c>
-      <c r="S30" s="29"/>
-      <c r="T30" s="50">
+      <c r="S30" s="19"/>
+      <c r="T30" s="9">
         <v>1</v>
       </c>
       <c r="U30" s="4">
@@ -1779,24 +1864,24 @@
       </c>
     </row>
     <row r="31" spans="2:22" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B31" s="11"/>
-      <c r="C31" s="12"/>
-      <c r="D31" s="26" t="s">
+      <c r="B31" s="32"/>
+      <c r="C31" s="33"/>
+      <c r="D31" s="20" t="s">
         <v>46</v>
       </c>
-      <c r="E31" s="27"/>
-      <c r="F31" s="51"/>
-      <c r="G31" s="58"/>
+      <c r="E31" s="21"/>
+      <c r="F31" s="10"/>
+      <c r="G31" s="3"/>
       <c r="H31" s="3"/>
-      <c r="I31" s="9" t="s">
+      <c r="I31" s="30" t="s">
         <v>26</v>
       </c>
-      <c r="J31" s="10"/>
-      <c r="K31" s="28" t="s">
+      <c r="J31" s="31"/>
+      <c r="K31" s="18" t="s">
         <v>5</v>
       </c>
-      <c r="L31" s="29"/>
-      <c r="M31" s="50">
+      <c r="L31" s="19"/>
+      <c r="M31" s="9">
         <v>1</v>
       </c>
       <c r="N31" s="4">
@@ -1804,73 +1889,73 @@
         <v>1</v>
       </c>
       <c r="O31" s="3"/>
-      <c r="P31" s="11"/>
-      <c r="Q31" s="12"/>
-      <c r="R31" s="26" t="s">
+      <c r="P31" s="32"/>
+      <c r="Q31" s="33"/>
+      <c r="R31" s="20" t="s">
         <v>47</v>
       </c>
-      <c r="S31" s="27"/>
-      <c r="T31" s="51">
+      <c r="S31" s="21"/>
+      <c r="T31" s="10">
         <v>1</v>
       </c>
       <c r="U31" s="3"/>
     </row>
     <row r="32" spans="2:22" x14ac:dyDescent="0.3">
-      <c r="B32" s="11"/>
-      <c r="C32" s="12"/>
-      <c r="D32" s="26" t="s">
+      <c r="B32" s="32"/>
+      <c r="C32" s="33"/>
+      <c r="D32" s="20" t="s">
         <v>10</v>
       </c>
-      <c r="E32" s="27"/>
-      <c r="F32" s="51">
-        <v>1</v>
-      </c>
-      <c r="G32" s="58"/>
+      <c r="E32" s="21"/>
+      <c r="F32" s="10">
+        <v>1</v>
+      </c>
+      <c r="G32" s="3"/>
       <c r="H32" s="3"/>
-      <c r="I32" s="11"/>
-      <c r="J32" s="12"/>
-      <c r="K32" s="26" t="s">
+      <c r="I32" s="32"/>
+      <c r="J32" s="33"/>
+      <c r="K32" s="20" t="s">
         <v>9</v>
       </c>
-      <c r="L32" s="27"/>
-      <c r="M32" s="51"/>
-      <c r="N32" s="58"/>
+      <c r="L32" s="21"/>
+      <c r="M32" s="10"/>
+      <c r="N32" s="3"/>
       <c r="O32" s="3"/>
-      <c r="P32" s="11"/>
-      <c r="Q32" s="12"/>
-      <c r="R32" s="26" t="s">
+      <c r="P32" s="32"/>
+      <c r="Q32" s="33"/>
+      <c r="R32" s="20" t="s">
         <v>15</v>
       </c>
-      <c r="S32" s="27"/>
-      <c r="T32" s="51"/>
+      <c r="S32" s="21"/>
+      <c r="T32" s="10"/>
       <c r="U32" s="3"/>
     </row>
     <row r="33" spans="1:22" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B33" s="13"/>
-      <c r="C33" s="14"/>
-      <c r="D33" s="56" t="s">
+      <c r="B33" s="34"/>
+      <c r="C33" s="35"/>
+      <c r="D33" s="28" t="s">
         <v>13</v>
       </c>
-      <c r="E33" s="57"/>
-      <c r="F33" s="52"/>
-      <c r="G33" s="58"/>
+      <c r="E33" s="29"/>
+      <c r="F33" s="11"/>
+      <c r="G33" s="3"/>
       <c r="H33" s="3"/>
-      <c r="I33" s="13"/>
-      <c r="J33" s="14"/>
-      <c r="K33" s="56" t="s">
+      <c r="I33" s="34"/>
+      <c r="J33" s="35"/>
+      <c r="K33" s="28" t="s">
         <v>15</v>
       </c>
-      <c r="L33" s="57"/>
-      <c r="M33" s="52"/>
-      <c r="N33" s="58"/>
+      <c r="L33" s="29"/>
+      <c r="M33" s="11"/>
+      <c r="N33" s="3"/>
       <c r="O33" s="3"/>
-      <c r="P33" s="11"/>
-      <c r="Q33" s="12"/>
-      <c r="R33" s="26" t="s">
+      <c r="P33" s="32"/>
+      <c r="Q33" s="33"/>
+      <c r="R33" s="20" t="s">
         <v>9</v>
       </c>
-      <c r="S33" s="27"/>
-      <c r="T33" s="51"/>
+      <c r="S33" s="21"/>
+      <c r="T33" s="10"/>
       <c r="U33" s="3"/>
     </row>
     <row r="34" spans="1:22" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -1888,13 +1973,13 @@
       <c r="M34" s="3"/>
       <c r="N34" s="3"/>
       <c r="O34" s="3"/>
-      <c r="P34" s="13"/>
-      <c r="Q34" s="14"/>
-      <c r="R34" s="56" t="s">
+      <c r="P34" s="34"/>
+      <c r="Q34" s="35"/>
+      <c r="R34" s="28" t="s">
         <v>12</v>
       </c>
-      <c r="S34" s="57"/>
-      <c r="T34" s="52"/>
+      <c r="S34" s="29"/>
+      <c r="T34" s="11"/>
       <c r="U34" s="3"/>
     </row>
     <row r="35" spans="1:22" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -1920,15 +2005,15 @@
       <c r="U35" s="3"/>
     </row>
     <row r="36" spans="1:22" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B36" s="9" t="s">
+      <c r="B36" s="30" t="s">
         <v>28</v>
       </c>
-      <c r="C36" s="10"/>
-      <c r="D36" s="28" t="s">
+      <c r="C36" s="31"/>
+      <c r="D36" s="18" t="s">
         <v>4</v>
       </c>
-      <c r="E36" s="29"/>
-      <c r="F36" s="50">
+      <c r="E36" s="19"/>
+      <c r="F36" s="9">
         <v>1</v>
       </c>
       <c r="G36" s="4">
@@ -1936,15 +2021,15 @@
         <v>2</v>
       </c>
       <c r="H36" s="3"/>
-      <c r="I36" s="9" t="s">
+      <c r="I36" s="30" t="s">
         <v>29</v>
       </c>
-      <c r="J36" s="19"/>
-      <c r="K36" s="28" t="s">
+      <c r="J36" s="36"/>
+      <c r="K36" s="18" t="s">
         <v>4</v>
       </c>
-      <c r="L36" s="29"/>
-      <c r="M36" s="50">
+      <c r="L36" s="19"/>
+      <c r="M36" s="9">
         <v>1</v>
       </c>
       <c r="N36" s="4">
@@ -1952,15 +2037,15 @@
         <v>1</v>
       </c>
       <c r="O36" s="3"/>
-      <c r="P36" s="9" t="s">
+      <c r="P36" s="30" t="s">
         <v>30</v>
       </c>
-      <c r="Q36" s="10"/>
-      <c r="R36" s="28" t="s">
+      <c r="Q36" s="31"/>
+      <c r="R36" s="18" t="s">
         <v>4</v>
       </c>
-      <c r="S36" s="29"/>
-      <c r="T36" s="50">
+      <c r="S36" s="19"/>
+      <c r="T36" s="9">
         <v>1</v>
       </c>
       <c r="U36" s="4">
@@ -1969,105 +2054,105 @@
       </c>
     </row>
     <row r="37" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="B37" s="11"/>
-      <c r="C37" s="12"/>
-      <c r="D37" s="26" t="s">
+      <c r="B37" s="32"/>
+      <c r="C37" s="33"/>
+      <c r="D37" s="20" t="s">
         <v>15</v>
       </c>
-      <c r="E37" s="27"/>
-      <c r="F37" s="51"/>
-      <c r="G37" s="58"/>
+      <c r="E37" s="21"/>
+      <c r="F37" s="10"/>
+      <c r="G37" s="3"/>
       <c r="H37" s="3"/>
-      <c r="I37" s="11"/>
-      <c r="J37" s="20"/>
-      <c r="K37" s="26" t="s">
+      <c r="I37" s="32"/>
+      <c r="J37" s="37"/>
+      <c r="K37" s="20" t="s">
         <v>15</v>
       </c>
-      <c r="L37" s="27"/>
-      <c r="M37" s="51"/>
-      <c r="N37" s="58"/>
+      <c r="L37" s="21"/>
+      <c r="M37" s="10"/>
+      <c r="N37" s="3"/>
       <c r="O37" s="3"/>
-      <c r="P37" s="11"/>
-      <c r="Q37" s="12"/>
-      <c r="R37" s="26" t="s">
+      <c r="P37" s="32"/>
+      <c r="Q37" s="33"/>
+      <c r="R37" s="20" t="s">
         <v>15</v>
       </c>
-      <c r="S37" s="27"/>
-      <c r="T37" s="51"/>
+      <c r="S37" s="21"/>
+      <c r="T37" s="10"/>
       <c r="U37" s="3"/>
     </row>
     <row r="38" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A38" s="1"/>
-      <c r="B38" s="11"/>
-      <c r="C38" s="12"/>
-      <c r="D38" s="26" t="s">
+      <c r="B38" s="32"/>
+      <c r="C38" s="33"/>
+      <c r="D38" s="20" t="s">
         <v>9</v>
       </c>
-      <c r="E38" s="27"/>
-      <c r="F38" s="51"/>
-      <c r="G38" s="58"/>
+      <c r="E38" s="21"/>
+      <c r="F38" s="10"/>
+      <c r="G38" s="3"/>
       <c r="H38" s="3"/>
-      <c r="I38" s="11"/>
-      <c r="J38" s="20"/>
-      <c r="K38" s="26" t="s">
+      <c r="I38" s="32"/>
+      <c r="J38" s="37"/>
+      <c r="K38" s="20" t="s">
         <v>9</v>
       </c>
-      <c r="L38" s="27"/>
-      <c r="M38" s="51"/>
-      <c r="N38" s="58"/>
+      <c r="L38" s="21"/>
+      <c r="M38" s="10"/>
+      <c r="N38" s="3"/>
       <c r="O38" s="3"/>
-      <c r="P38" s="11"/>
-      <c r="Q38" s="12"/>
-      <c r="R38" s="26" t="s">
+      <c r="P38" s="32"/>
+      <c r="Q38" s="33"/>
+      <c r="R38" s="20" t="s">
         <v>7</v>
       </c>
-      <c r="S38" s="27"/>
-      <c r="T38" s="51">
+      <c r="S38" s="21"/>
+      <c r="T38" s="10">
         <v>1</v>
       </c>
       <c r="U38" s="3"/>
     </row>
     <row r="39" spans="1:22" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A39" s="1"/>
-      <c r="B39" s="11"/>
-      <c r="C39" s="12"/>
-      <c r="D39" s="26" t="s">
+      <c r="B39" s="32"/>
+      <c r="C39" s="33"/>
+      <c r="D39" s="20" t="s">
         <v>12</v>
       </c>
-      <c r="E39" s="27"/>
-      <c r="F39" s="51"/>
-      <c r="G39" s="58"/>
+      <c r="E39" s="21"/>
+      <c r="F39" s="10"/>
+      <c r="G39" s="3"/>
       <c r="H39" s="3"/>
-      <c r="I39" s="13"/>
-      <c r="J39" s="21"/>
-      <c r="K39" s="56" t="s">
+      <c r="I39" s="34"/>
+      <c r="J39" s="38"/>
+      <c r="K39" s="28" t="s">
         <v>12</v>
       </c>
-      <c r="L39" s="57"/>
-      <c r="M39" s="52"/>
-      <c r="N39" s="58"/>
+      <c r="L39" s="29"/>
+      <c r="M39" s="11"/>
+      <c r="N39" s="3"/>
       <c r="O39" s="3"/>
-      <c r="P39" s="11"/>
-      <c r="Q39" s="12"/>
-      <c r="R39" s="26" t="s">
+      <c r="P39" s="32"/>
+      <c r="Q39" s="33"/>
+      <c r="R39" s="20" t="s">
         <v>9</v>
       </c>
-      <c r="S39" s="27"/>
-      <c r="T39" s="51"/>
+      <c r="S39" s="21"/>
+      <c r="T39" s="10"/>
       <c r="U39" s="3"/>
     </row>
     <row r="40" spans="1:22" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A40" s="1"/>
-      <c r="B40" s="13"/>
-      <c r="C40" s="14"/>
-      <c r="D40" s="56" t="s">
+      <c r="B40" s="34"/>
+      <c r="C40" s="35"/>
+      <c r="D40" s="28" t="s">
         <v>49</v>
       </c>
-      <c r="E40" s="57"/>
-      <c r="F40" s="52">
-        <v>1</v>
-      </c>
-      <c r="G40" s="58"/>
+      <c r="E40" s="29"/>
+      <c r="F40" s="11">
+        <v>1</v>
+      </c>
+      <c r="G40" s="3"/>
       <c r="H40" s="3"/>
       <c r="I40" s="3"/>
       <c r="J40" s="3"/>
@@ -2076,13 +2161,13 @@
       <c r="M40" s="3"/>
       <c r="N40" s="3"/>
       <c r="O40" s="3"/>
-      <c r="P40" s="11"/>
-      <c r="Q40" s="12"/>
-      <c r="R40" s="26" t="s">
+      <c r="P40" s="32"/>
+      <c r="Q40" s="33"/>
+      <c r="R40" s="20" t="s">
         <v>8</v>
       </c>
-      <c r="S40" s="27"/>
-      <c r="T40" s="51"/>
+      <c r="S40" s="21"/>
+      <c r="T40" s="10"/>
       <c r="U40" s="3"/>
       <c r="V40" s="1"/>
     </row>
@@ -2102,13 +2187,13 @@
       <c r="M41" s="3"/>
       <c r="N41" s="3"/>
       <c r="O41" s="3"/>
-      <c r="P41" s="11"/>
-      <c r="Q41" s="12"/>
-      <c r="R41" s="26" t="s">
+      <c r="P41" s="32"/>
+      <c r="Q41" s="33"/>
+      <c r="R41" s="20" t="s">
         <v>6</v>
       </c>
-      <c r="S41" s="27"/>
-      <c r="T41" s="51">
+      <c r="S41" s="21"/>
+      <c r="T41" s="10">
         <v>1</v>
       </c>
       <c r="U41" s="3"/>
@@ -2130,28 +2215,28 @@
       <c r="M42" s="3"/>
       <c r="N42" s="3"/>
       <c r="O42" s="3"/>
-      <c r="P42" s="11"/>
-      <c r="Q42" s="12"/>
-      <c r="R42" s="26" t="s">
+      <c r="P42" s="32"/>
+      <c r="Q42" s="33"/>
+      <c r="R42" s="20" t="s">
         <v>10</v>
       </c>
-      <c r="S42" s="27"/>
-      <c r="T42" s="51">
+      <c r="S42" s="21"/>
+      <c r="T42" s="10">
         <v>1</v>
       </c>
       <c r="U42" s="3"/>
       <c r="V42" s="1"/>
     </row>
     <row r="43" spans="1:22" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B43" s="9" t="s">
+      <c r="B43" s="30" t="s">
         <v>31</v>
       </c>
-      <c r="C43" s="19"/>
-      <c r="D43" s="28" t="s">
+      <c r="C43" s="36"/>
+      <c r="D43" s="18" t="s">
         <v>4</v>
       </c>
-      <c r="E43" s="29"/>
-      <c r="F43" s="50">
+      <c r="E43" s="19"/>
+      <c r="F43" s="9">
         <v>1</v>
       </c>
       <c r="G43" s="4">
@@ -2159,15 +2244,15 @@
         <v>3</v>
       </c>
       <c r="H43" s="3"/>
-      <c r="I43" s="9" t="s">
+      <c r="I43" s="30" t="s">
         <v>32</v>
       </c>
-      <c r="J43" s="10"/>
-      <c r="K43" s="28" t="s">
+      <c r="J43" s="31"/>
+      <c r="K43" s="18" t="s">
         <v>5</v>
       </c>
-      <c r="L43" s="29"/>
-      <c r="M43" s="50">
+      <c r="L43" s="19"/>
+      <c r="M43" s="9">
         <v>1</v>
       </c>
       <c r="N43" s="4">
@@ -2175,36 +2260,36 @@
         <v>4</v>
       </c>
       <c r="O43" s="3"/>
-      <c r="P43" s="13"/>
-      <c r="Q43" s="14"/>
-      <c r="R43" s="56" t="s">
+      <c r="P43" s="34"/>
+      <c r="Q43" s="35"/>
+      <c r="R43" s="28" t="s">
         <v>12</v>
       </c>
-      <c r="S43" s="57"/>
-      <c r="T43" s="52"/>
+      <c r="S43" s="29"/>
+      <c r="T43" s="11"/>
       <c r="U43" s="3"/>
       <c r="V43" s="1"/>
     </row>
     <row r="44" spans="1:22" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B44" s="11"/>
-      <c r="C44" s="20"/>
-      <c r="D44" s="26" t="s">
+      <c r="B44" s="32"/>
+      <c r="C44" s="37"/>
+      <c r="D44" s="20" t="s">
         <v>15</v>
       </c>
-      <c r="E44" s="27"/>
-      <c r="F44" s="51"/>
-      <c r="G44" s="58"/>
+      <c r="E44" s="21"/>
+      <c r="F44" s="10"/>
+      <c r="G44" s="3"/>
       <c r="H44" s="3"/>
-      <c r="I44" s="11"/>
-      <c r="J44" s="12"/>
-      <c r="K44" s="26" t="s">
+      <c r="I44" s="32"/>
+      <c r="J44" s="33"/>
+      <c r="K44" s="20" t="s">
         <v>6</v>
       </c>
-      <c r="L44" s="27"/>
-      <c r="M44" s="51">
-        <v>1</v>
-      </c>
-      <c r="N44" s="58"/>
+      <c r="L44" s="21"/>
+      <c r="M44" s="10">
+        <v>1</v>
+      </c>
+      <c r="N44" s="3"/>
       <c r="O44" s="3"/>
       <c r="P44" s="3"/>
       <c r="Q44" s="3"/>
@@ -2215,33 +2300,33 @@
       <c r="V44" s="1"/>
     </row>
     <row r="45" spans="1:22" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B45" s="11"/>
-      <c r="C45" s="20"/>
-      <c r="D45" s="26" t="s">
+      <c r="B45" s="32"/>
+      <c r="C45" s="37"/>
+      <c r="D45" s="20" t="s">
         <v>9</v>
       </c>
-      <c r="E45" s="27"/>
-      <c r="F45" s="51"/>
-      <c r="G45" s="58"/>
+      <c r="E45" s="21"/>
+      <c r="F45" s="10"/>
+      <c r="G45" s="3"/>
       <c r="H45" s="3"/>
-      <c r="I45" s="11"/>
-      <c r="J45" s="12"/>
-      <c r="K45" s="26" t="s">
+      <c r="I45" s="32"/>
+      <c r="J45" s="33"/>
+      <c r="K45" s="20" t="s">
         <v>15</v>
       </c>
-      <c r="L45" s="27"/>
-      <c r="M45" s="51"/>
-      <c r="N45" s="58"/>
+      <c r="L45" s="21"/>
+      <c r="M45" s="10"/>
+      <c r="N45" s="3"/>
       <c r="O45" s="3"/>
-      <c r="P45" s="9" t="s">
+      <c r="P45" s="30" t="s">
         <v>34</v>
       </c>
-      <c r="Q45" s="10"/>
-      <c r="R45" s="28" t="s">
+      <c r="Q45" s="31"/>
+      <c r="R45" s="18" t="s">
         <v>8</v>
       </c>
-      <c r="S45" s="29"/>
-      <c r="T45" s="50"/>
+      <c r="S45" s="19"/>
+      <c r="T45" s="9"/>
       <c r="U45" s="4">
         <f>SUM(T45:T55)</f>
         <v>5</v>
@@ -2249,68 +2334,68 @@
       <c r="V45" s="1"/>
     </row>
     <row r="46" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="B46" s="11"/>
-      <c r="C46" s="20"/>
-      <c r="D46" s="26" t="s">
+      <c r="B46" s="32"/>
+      <c r="C46" s="37"/>
+      <c r="D46" s="20" t="s">
         <v>50</v>
       </c>
-      <c r="E46" s="27"/>
-      <c r="F46" s="51">
-        <v>1</v>
-      </c>
-      <c r="G46" s="58"/>
+      <c r="E46" s="21"/>
+      <c r="F46" s="10">
+        <v>1</v>
+      </c>
+      <c r="G46" s="3"/>
       <c r="H46" s="3"/>
-      <c r="I46" s="11"/>
-      <c r="J46" s="12"/>
-      <c r="K46" s="26" t="s">
+      <c r="I46" s="32"/>
+      <c r="J46" s="33"/>
+      <c r="K46" s="20" t="s">
         <v>8</v>
       </c>
-      <c r="L46" s="27"/>
-      <c r="M46" s="51"/>
-      <c r="N46" s="58"/>
+      <c r="L46" s="21"/>
+      <c r="M46" s="10"/>
+      <c r="N46" s="3"/>
       <c r="O46" s="3"/>
-      <c r="P46" s="11"/>
-      <c r="Q46" s="12"/>
-      <c r="R46" s="26" t="s">
+      <c r="P46" s="32"/>
+      <c r="Q46" s="33"/>
+      <c r="R46" s="20" t="s">
         <v>10</v>
       </c>
-      <c r="S46" s="27"/>
-      <c r="T46" s="51">
+      <c r="S46" s="21"/>
+      <c r="T46" s="10">
         <v>1</v>
       </c>
       <c r="U46" s="3"/>
       <c r="V46" s="1"/>
     </row>
     <row r="47" spans="1:22" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B47" s="13"/>
-      <c r="C47" s="21"/>
-      <c r="D47" s="56" t="s">
+      <c r="B47" s="34"/>
+      <c r="C47" s="38"/>
+      <c r="D47" s="28" t="s">
         <v>49</v>
       </c>
-      <c r="E47" s="57"/>
-      <c r="F47" s="52">
-        <v>1</v>
-      </c>
-      <c r="G47" s="58"/>
+      <c r="E47" s="29"/>
+      <c r="F47" s="11">
+        <v>1</v>
+      </c>
+      <c r="G47" s="3"/>
       <c r="H47" s="3"/>
-      <c r="I47" s="11"/>
-      <c r="J47" s="12"/>
-      <c r="K47" s="26" t="s">
+      <c r="I47" s="32"/>
+      <c r="J47" s="33"/>
+      <c r="K47" s="20" t="s">
         <v>10</v>
       </c>
-      <c r="L47" s="27"/>
-      <c r="M47" s="51">
-        <v>1</v>
-      </c>
-      <c r="N47" s="58"/>
+      <c r="L47" s="21"/>
+      <c r="M47" s="10">
+        <v>1</v>
+      </c>
+      <c r="N47" s="3"/>
       <c r="O47" s="3"/>
-      <c r="P47" s="11"/>
-      <c r="Q47" s="12"/>
-      <c r="R47" s="26" t="s">
+      <c r="P47" s="32"/>
+      <c r="Q47" s="33"/>
+      <c r="R47" s="20" t="s">
         <v>7</v>
       </c>
-      <c r="S47" s="27"/>
-      <c r="T47" s="51">
+      <c r="S47" s="21"/>
+      <c r="T47" s="10">
         <v>1</v>
       </c>
       <c r="U47" s="3"/>
@@ -2324,25 +2409,25 @@
       <c r="F48" s="3"/>
       <c r="G48" s="3"/>
       <c r="H48" s="3"/>
-      <c r="I48" s="13"/>
-      <c r="J48" s="14"/>
-      <c r="K48" s="17" t="s">
+      <c r="I48" s="34"/>
+      <c r="J48" s="35"/>
+      <c r="K48" s="39" t="s">
         <v>53</v>
       </c>
-      <c r="L48" s="18"/>
-      <c r="M48" s="52">
+      <c r="L48" s="40"/>
+      <c r="M48" s="11">
         <f>4-3</f>
         <v>1</v>
       </c>
-      <c r="N48" s="58"/>
+      <c r="N48" s="3"/>
       <c r="O48" s="3"/>
-      <c r="P48" s="11"/>
-      <c r="Q48" s="12"/>
-      <c r="R48" s="26" t="s">
+      <c r="P48" s="32"/>
+      <c r="Q48" s="33"/>
+      <c r="R48" s="20" t="s">
         <v>6</v>
       </c>
-      <c r="S48" s="27"/>
-      <c r="T48" s="51">
+      <c r="S48" s="21"/>
+      <c r="T48" s="10">
         <v>1</v>
       </c>
       <c r="U48" s="3"/>
@@ -2363,26 +2448,26 @@
       <c r="M49" s="3"/>
       <c r="N49" s="3"/>
       <c r="O49" s="3"/>
-      <c r="P49" s="11"/>
-      <c r="Q49" s="12"/>
-      <c r="R49" s="26" t="s">
+      <c r="P49" s="32"/>
+      <c r="Q49" s="33"/>
+      <c r="R49" s="20" t="s">
         <v>54</v>
       </c>
-      <c r="S49" s="27"/>
-      <c r="T49" s="51"/>
+      <c r="S49" s="21"/>
+      <c r="T49" s="10"/>
       <c r="U49" s="3"/>
       <c r="V49" s="1"/>
     </row>
     <row r="50" spans="2:22" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B50" s="9" t="s">
+      <c r="B50" s="30" t="s">
         <v>33</v>
       </c>
-      <c r="C50" s="10"/>
-      <c r="D50" s="28" t="s">
+      <c r="C50" s="31"/>
+      <c r="D50" s="18" t="s">
         <v>4</v>
       </c>
-      <c r="E50" s="29"/>
-      <c r="F50" s="50">
+      <c r="E50" s="19"/>
+      <c r="F50" s="9">
         <v>1</v>
       </c>
       <c r="G50" s="4">
@@ -2390,15 +2475,15 @@
         <v>5</v>
       </c>
       <c r="H50" s="3"/>
-      <c r="I50" s="9" t="s">
+      <c r="I50" s="30" t="s">
         <v>35</v>
       </c>
-      <c r="J50" s="10"/>
-      <c r="K50" s="28" t="s">
+      <c r="J50" s="31"/>
+      <c r="K50" s="18" t="s">
         <v>4</v>
       </c>
-      <c r="L50" s="29"/>
-      <c r="M50" s="50">
+      <c r="L50" s="19"/>
+      <c r="M50" s="9">
         <v>1</v>
       </c>
       <c r="N50" s="4">
@@ -2406,168 +2491,168 @@
         <v>4</v>
       </c>
       <c r="O50" s="3"/>
-      <c r="P50" s="11"/>
-      <c r="Q50" s="12"/>
-      <c r="R50" s="26" t="s">
+      <c r="P50" s="32"/>
+      <c r="Q50" s="33"/>
+      <c r="R50" s="20" t="s">
         <v>45</v>
       </c>
-      <c r="S50" s="27"/>
-      <c r="T50" s="51"/>
+      <c r="S50" s="21"/>
+      <c r="T50" s="10"/>
       <c r="U50" s="3"/>
       <c r="V50" s="1"/>
     </row>
     <row r="51" spans="2:22" x14ac:dyDescent="0.3">
-      <c r="B51" s="11"/>
-      <c r="C51" s="12"/>
-      <c r="D51" s="26" t="s">
+      <c r="B51" s="32"/>
+      <c r="C51" s="33"/>
+      <c r="D51" s="20" t="s">
         <v>10</v>
       </c>
-      <c r="E51" s="27"/>
-      <c r="F51" s="51">
-        <v>1</v>
-      </c>
-      <c r="G51" s="58"/>
+      <c r="E51" s="21"/>
+      <c r="F51" s="10">
+        <v>1</v>
+      </c>
+      <c r="G51" s="3"/>
       <c r="H51" s="3"/>
-      <c r="I51" s="11"/>
-      <c r="J51" s="12"/>
-      <c r="K51" s="26" t="s">
+      <c r="I51" s="32"/>
+      <c r="J51" s="33"/>
+      <c r="K51" s="20" t="s">
         <v>10</v>
       </c>
-      <c r="L51" s="27"/>
-      <c r="M51" s="51">
-        <v>1</v>
-      </c>
-      <c r="N51" s="58"/>
+      <c r="L51" s="21"/>
+      <c r="M51" s="10">
+        <v>1</v>
+      </c>
+      <c r="N51" s="3"/>
       <c r="O51" s="3"/>
-      <c r="P51" s="11"/>
-      <c r="Q51" s="12"/>
-      <c r="R51" s="26" t="s">
+      <c r="P51" s="32"/>
+      <c r="Q51" s="33"/>
+      <c r="R51" s="20" t="s">
         <v>17</v>
       </c>
-      <c r="S51" s="27"/>
-      <c r="T51" s="51"/>
+      <c r="S51" s="21"/>
+      <c r="T51" s="10"/>
       <c r="U51" s="3"/>
       <c r="V51" s="1"/>
     </row>
     <row r="52" spans="2:22" x14ac:dyDescent="0.3">
-      <c r="B52" s="11"/>
-      <c r="C52" s="12"/>
-      <c r="D52" s="26" t="s">
+      <c r="B52" s="32"/>
+      <c r="C52" s="33"/>
+      <c r="D52" s="20" t="s">
         <v>6</v>
       </c>
-      <c r="E52" s="27"/>
-      <c r="F52" s="51">
-        <v>1</v>
-      </c>
-      <c r="G52" s="58"/>
+      <c r="E52" s="21"/>
+      <c r="F52" s="10">
+        <v>1</v>
+      </c>
+      <c r="G52" s="3"/>
       <c r="H52" s="3"/>
-      <c r="I52" s="11"/>
-      <c r="J52" s="12"/>
-      <c r="K52" s="26" t="s">
+      <c r="I52" s="32"/>
+      <c r="J52" s="33"/>
+      <c r="K52" s="20" t="s">
         <v>15</v>
       </c>
-      <c r="L52" s="27"/>
-      <c r="M52" s="51"/>
-      <c r="N52" s="58"/>
+      <c r="L52" s="21"/>
+      <c r="M52" s="10"/>
+      <c r="N52" s="3"/>
       <c r="O52" s="3"/>
-      <c r="P52" s="11"/>
-      <c r="Q52" s="12"/>
-      <c r="R52" s="26" t="s">
+      <c r="P52" s="32"/>
+      <c r="Q52" s="33"/>
+      <c r="R52" s="20" t="s">
         <v>59</v>
       </c>
-      <c r="S52" s="27"/>
-      <c r="T52" s="51">
+      <c r="S52" s="21"/>
+      <c r="T52" s="10">
         <v>1</v>
       </c>
       <c r="U52" s="3"/>
       <c r="V52" s="1"/>
     </row>
     <row r="53" spans="2:22" x14ac:dyDescent="0.3">
-      <c r="B53" s="11"/>
-      <c r="C53" s="12"/>
-      <c r="D53" s="26" t="s">
+      <c r="B53" s="32"/>
+      <c r="C53" s="33"/>
+      <c r="D53" s="20" t="s">
         <v>15</v>
       </c>
-      <c r="E53" s="27"/>
-      <c r="F53" s="51"/>
-      <c r="G53" s="58"/>
+      <c r="E53" s="21"/>
+      <c r="F53" s="10"/>
+      <c r="G53" s="3"/>
       <c r="H53" s="3"/>
-      <c r="I53" s="11"/>
-      <c r="J53" s="12"/>
-      <c r="K53" s="26" t="s">
+      <c r="I53" s="32"/>
+      <c r="J53" s="33"/>
+      <c r="K53" s="20" t="s">
         <v>8</v>
       </c>
-      <c r="L53" s="27"/>
-      <c r="M53" s="51"/>
-      <c r="N53" s="58"/>
+      <c r="L53" s="21"/>
+      <c r="M53" s="10"/>
+      <c r="N53" s="3"/>
       <c r="O53" s="3"/>
-      <c r="P53" s="11"/>
-      <c r="Q53" s="12"/>
-      <c r="R53" s="26" t="s">
+      <c r="P53" s="32"/>
+      <c r="Q53" s="33"/>
+      <c r="R53" s="20" t="s">
         <v>60</v>
       </c>
-      <c r="S53" s="27"/>
-      <c r="T53" s="51"/>
+      <c r="S53" s="21"/>
+      <c r="T53" s="10"/>
       <c r="U53" s="3"/>
       <c r="V53" s="1"/>
     </row>
     <row r="54" spans="2:22" x14ac:dyDescent="0.3">
-      <c r="B54" s="11"/>
-      <c r="C54" s="12"/>
-      <c r="D54" s="26" t="s">
+      <c r="B54" s="32"/>
+      <c r="C54" s="33"/>
+      <c r="D54" s="20" t="s">
         <v>8</v>
       </c>
-      <c r="E54" s="27"/>
-      <c r="F54" s="51"/>
-      <c r="G54" s="58"/>
+      <c r="E54" s="21"/>
+      <c r="F54" s="10"/>
+      <c r="G54" s="3"/>
       <c r="H54" s="3"/>
-      <c r="I54" s="11"/>
-      <c r="J54" s="12"/>
-      <c r="K54" s="26" t="s">
+      <c r="I54" s="32"/>
+      <c r="J54" s="33"/>
+      <c r="K54" s="20" t="s">
         <v>13</v>
       </c>
-      <c r="L54" s="27"/>
-      <c r="M54" s="51"/>
-      <c r="N54" s="58"/>
+      <c r="L54" s="21"/>
+      <c r="M54" s="10"/>
+      <c r="N54" s="3"/>
       <c r="O54" s="3"/>
-      <c r="P54" s="11"/>
-      <c r="Q54" s="12"/>
-      <c r="R54" s="26" t="s">
+      <c r="P54" s="32"/>
+      <c r="Q54" s="33"/>
+      <c r="R54" s="20" t="s">
         <v>61</v>
       </c>
-      <c r="S54" s="27"/>
-      <c r="T54" s="51"/>
+      <c r="S54" s="21"/>
+      <c r="T54" s="10"/>
       <c r="U54" s="3"/>
       <c r="V54" s="1"/>
     </row>
     <row r="55" spans="2:22" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B55" s="11"/>
-      <c r="C55" s="12"/>
-      <c r="D55" s="26" t="s">
+      <c r="B55" s="32"/>
+      <c r="C55" s="33"/>
+      <c r="D55" s="20" t="s">
         <v>14</v>
       </c>
-      <c r="E55" s="27"/>
-      <c r="F55" s="51">
-        <v>1</v>
-      </c>
-      <c r="G55" s="58"/>
+      <c r="E55" s="21"/>
+      <c r="F55" s="10">
+        <v>1</v>
+      </c>
+      <c r="G55" s="3"/>
       <c r="H55" s="3"/>
-      <c r="I55" s="11"/>
-      <c r="J55" s="12"/>
-      <c r="K55" s="26" t="s">
+      <c r="I55" s="32"/>
+      <c r="J55" s="33"/>
+      <c r="K55" s="20" t="s">
         <v>62</v>
       </c>
-      <c r="L55" s="27"/>
-      <c r="M55" s="51"/>
-      <c r="N55" s="58"/>
+      <c r="L55" s="21"/>
+      <c r="M55" s="10"/>
+      <c r="N55" s="3"/>
       <c r="O55" s="3"/>
-      <c r="P55" s="13"/>
-      <c r="Q55" s="14"/>
-      <c r="R55" s="17" t="s">
+      <c r="P55" s="34"/>
+      <c r="Q55" s="35"/>
+      <c r="R55" s="39" t="s">
         <v>58</v>
       </c>
-      <c r="S55" s="18"/>
-      <c r="T55" s="52">
+      <c r="S55" s="40"/>
+      <c r="T55" s="11">
         <f>2-1</f>
         <v>1</v>
       </c>
@@ -2575,28 +2660,28 @@
       <c r="V55" s="1"/>
     </row>
     <row r="56" spans="2:22" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B56" s="13"/>
-      <c r="C56" s="14"/>
-      <c r="D56" s="17" t="s">
+      <c r="B56" s="34"/>
+      <c r="C56" s="35"/>
+      <c r="D56" s="39" t="s">
         <v>57</v>
       </c>
-      <c r="E56" s="18"/>
-      <c r="F56" s="52">
+      <c r="E56" s="40"/>
+      <c r="F56" s="11">
         <f>3-2</f>
         <v>1</v>
       </c>
-      <c r="G56" s="58"/>
+      <c r="G56" s="3"/>
       <c r="H56" s="3"/>
-      <c r="I56" s="11"/>
-      <c r="J56" s="12"/>
-      <c r="K56" s="26" t="s">
+      <c r="I56" s="32"/>
+      <c r="J56" s="33"/>
+      <c r="K56" s="20" t="s">
         <v>6</v>
       </c>
-      <c r="L56" s="27"/>
-      <c r="M56" s="51">
-        <v>1</v>
-      </c>
-      <c r="N56" s="58"/>
+      <c r="L56" s="21"/>
+      <c r="M56" s="10">
+        <v>1</v>
+      </c>
+      <c r="N56" s="3"/>
       <c r="O56" s="3"/>
       <c r="P56" s="3"/>
       <c r="Q56" s="3"/>
@@ -2614,26 +2699,26 @@
       <c r="F57" s="3"/>
       <c r="G57" s="3"/>
       <c r="H57" s="3"/>
-      <c r="I57" s="13"/>
-      <c r="J57" s="14"/>
-      <c r="K57" s="56" t="s">
+      <c r="I57" s="34"/>
+      <c r="J57" s="35"/>
+      <c r="K57" s="28" t="s">
         <v>7</v>
       </c>
-      <c r="L57" s="57"/>
-      <c r="M57" s="52">
-        <v>1</v>
-      </c>
-      <c r="N57" s="58"/>
+      <c r="L57" s="29"/>
+      <c r="M57" s="11">
+        <v>1</v>
+      </c>
+      <c r="N57" s="3"/>
       <c r="O57" s="3"/>
-      <c r="P57" s="9" t="s">
+      <c r="P57" s="30" t="s">
         <v>38</v>
       </c>
-      <c r="Q57" s="10"/>
-      <c r="R57" s="28" t="s">
+      <c r="Q57" s="31"/>
+      <c r="R57" s="18" t="s">
         <v>7</v>
       </c>
-      <c r="S57" s="29"/>
-      <c r="T57" s="50">
+      <c r="S57" s="19"/>
+      <c r="T57" s="9">
         <v>1</v>
       </c>
       <c r="U57" s="4">
@@ -2656,13 +2741,13 @@
       <c r="M58" s="3"/>
       <c r="N58" s="3"/>
       <c r="O58" s="3"/>
-      <c r="P58" s="11"/>
-      <c r="Q58" s="12"/>
-      <c r="R58" s="26" t="s">
+      <c r="P58" s="32"/>
+      <c r="Q58" s="33"/>
+      <c r="R58" s="20" t="s">
         <v>17</v>
       </c>
-      <c r="S58" s="27"/>
-      <c r="T58" s="51"/>
+      <c r="S58" s="21"/>
+      <c r="T58" s="10"/>
       <c r="U58" s="3"/>
     </row>
     <row r="59" spans="2:22" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -2680,76 +2765,76 @@
       <c r="M59" s="3"/>
       <c r="N59" s="3"/>
       <c r="O59" s="3"/>
-      <c r="P59" s="11"/>
-      <c r="Q59" s="12"/>
-      <c r="R59" s="30" t="s">
+      <c r="P59" s="32"/>
+      <c r="Q59" s="33"/>
+      <c r="R59" s="42" t="s">
         <v>53</v>
       </c>
-      <c r="S59" s="31"/>
-      <c r="T59" s="51">
+      <c r="S59" s="43"/>
+      <c r="T59" s="10">
         <f>4-4</f>
         <v>0</v>
       </c>
       <c r="U59" s="3"/>
     </row>
     <row r="60" spans="2:22" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B60" s="9" t="s">
+      <c r="B60" s="30" t="s">
         <v>36</v>
       </c>
-      <c r="C60" s="10"/>
-      <c r="D60" s="28" t="s">
+      <c r="C60" s="31"/>
+      <c r="D60" s="18" t="s">
         <v>17</v>
       </c>
-      <c r="E60" s="29"/>
-      <c r="F60" s="50"/>
+      <c r="E60" s="19"/>
+      <c r="F60" s="9"/>
       <c r="G60" s="4">
         <f>SUM(F60:F66)</f>
         <v>4</v>
       </c>
       <c r="H60" s="3"/>
-      <c r="I60" s="9" t="s">
+      <c r="I60" s="30" t="s">
         <v>37</v>
       </c>
-      <c r="J60" s="10"/>
-      <c r="K60" s="28" t="s">
+      <c r="J60" s="31"/>
+      <c r="K60" s="18" t="s">
         <v>8</v>
       </c>
-      <c r="L60" s="29"/>
-      <c r="M60" s="50"/>
+      <c r="L60" s="19"/>
+      <c r="M60" s="9"/>
       <c r="N60" s="4">
         <f>SUM(M60:M66)</f>
         <v>4</v>
       </c>
       <c r="O60" s="3"/>
-      <c r="P60" s="13"/>
-      <c r="Q60" s="14"/>
-      <c r="R60" s="17" t="s">
+      <c r="P60" s="34"/>
+      <c r="Q60" s="35"/>
+      <c r="R60" s="39" t="s">
         <v>63</v>
       </c>
-      <c r="S60" s="18"/>
-      <c r="T60" s="52">
+      <c r="S60" s="40"/>
+      <c r="T60" s="11">
         <v>3</v>
       </c>
       <c r="U60" s="3"/>
     </row>
     <row r="61" spans="2:22" x14ac:dyDescent="0.3">
-      <c r="B61" s="11"/>
-      <c r="C61" s="12"/>
-      <c r="D61" s="26" t="s">
+      <c r="B61" s="32"/>
+      <c r="C61" s="33"/>
+      <c r="D61" s="20" t="s">
         <v>11</v>
       </c>
-      <c r="E61" s="27"/>
-      <c r="F61" s="51"/>
-      <c r="G61" s="58"/>
+      <c r="E61" s="21"/>
+      <c r="F61" s="10"/>
+      <c r="G61" s="3"/>
       <c r="H61" s="3"/>
-      <c r="I61" s="11"/>
-      <c r="J61" s="12"/>
-      <c r="K61" s="26" t="s">
+      <c r="I61" s="32"/>
+      <c r="J61" s="33"/>
+      <c r="K61" s="20" t="s">
         <v>13</v>
       </c>
-      <c r="L61" s="27"/>
-      <c r="M61" s="51"/>
-      <c r="N61" s="58"/>
+      <c r="L61" s="21"/>
+      <c r="M61" s="10"/>
+      <c r="N61" s="3"/>
       <c r="O61" s="3"/>
       <c r="P61" s="3"/>
       <c r="Q61" s="3"/>
@@ -2759,27 +2844,27 @@
       <c r="U61" s="3"/>
     </row>
     <row r="62" spans="2:22" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B62" s="11"/>
-      <c r="C62" s="12"/>
-      <c r="D62" s="26" t="s">
+      <c r="B62" s="32"/>
+      <c r="C62" s="33"/>
+      <c r="D62" s="20" t="s">
         <v>4</v>
       </c>
-      <c r="E62" s="27"/>
-      <c r="F62" s="51">
-        <v>1</v>
-      </c>
-      <c r="G62" s="58"/>
+      <c r="E62" s="21"/>
+      <c r="F62" s="10">
+        <v>1</v>
+      </c>
+      <c r="G62" s="3"/>
       <c r="H62" s="3"/>
-      <c r="I62" s="11"/>
-      <c r="J62" s="12"/>
-      <c r="K62" s="26" t="s">
+      <c r="I62" s="32"/>
+      <c r="J62" s="33"/>
+      <c r="K62" s="20" t="s">
         <v>4</v>
       </c>
-      <c r="L62" s="27"/>
-      <c r="M62" s="51">
-        <v>1</v>
-      </c>
-      <c r="N62" s="58"/>
+      <c r="L62" s="21"/>
+      <c r="M62" s="10">
+        <v>1</v>
+      </c>
+      <c r="N62" s="3"/>
       <c r="O62" s="3"/>
       <c r="P62" s="3"/>
       <c r="Q62" s="3"/>
@@ -2789,35 +2874,35 @@
       <c r="U62" s="3"/>
     </row>
     <row r="63" spans="2:22" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B63" s="11"/>
-      <c r="C63" s="12"/>
-      <c r="D63" s="26" t="s">
+      <c r="B63" s="32"/>
+      <c r="C63" s="33"/>
+      <c r="D63" s="20" t="s">
         <v>10</v>
       </c>
-      <c r="E63" s="27"/>
-      <c r="F63" s="51">
-        <v>1</v>
-      </c>
-      <c r="G63" s="58"/>
+      <c r="E63" s="21"/>
+      <c r="F63" s="10">
+        <v>1</v>
+      </c>
+      <c r="G63" s="3"/>
       <c r="H63" s="3"/>
-      <c r="I63" s="11"/>
-      <c r="J63" s="12"/>
-      <c r="K63" s="26" t="s">
+      <c r="I63" s="32"/>
+      <c r="J63" s="33"/>
+      <c r="K63" s="20" t="s">
         <v>15</v>
       </c>
-      <c r="L63" s="27"/>
-      <c r="M63" s="51"/>
-      <c r="N63" s="58"/>
+      <c r="L63" s="21"/>
+      <c r="M63" s="10"/>
+      <c r="N63" s="3"/>
       <c r="O63" s="3"/>
-      <c r="P63" s="9" t="s">
+      <c r="P63" s="30" t="s">
         <v>64</v>
       </c>
-      <c r="Q63" s="10"/>
-      <c r="R63" s="28" t="s">
+      <c r="Q63" s="31"/>
+      <c r="R63" s="18" t="s">
         <v>65</v>
       </c>
-      <c r="S63" s="29"/>
-      <c r="T63" s="50">
+      <c r="S63" s="19"/>
+      <c r="T63" s="9">
         <v>1</v>
       </c>
       <c r="U63" s="4">
@@ -2826,97 +2911,97 @@
       </c>
     </row>
     <row r="64" spans="2:22" x14ac:dyDescent="0.3">
-      <c r="B64" s="11"/>
-      <c r="C64" s="12"/>
-      <c r="D64" s="26" t="s">
+      <c r="B64" s="32"/>
+      <c r="C64" s="33"/>
+      <c r="D64" s="20" t="s">
         <v>15</v>
       </c>
-      <c r="E64" s="27"/>
-      <c r="F64" s="51"/>
-      <c r="G64" s="58"/>
+      <c r="E64" s="21"/>
+      <c r="F64" s="10"/>
+      <c r="G64" s="3"/>
       <c r="H64" s="3"/>
-      <c r="I64" s="11"/>
-      <c r="J64" s="12"/>
-      <c r="K64" s="26" t="s">
+      <c r="I64" s="32"/>
+      <c r="J64" s="33"/>
+      <c r="K64" s="20" t="s">
         <v>7</v>
       </c>
-      <c r="L64" s="27"/>
-      <c r="M64" s="51">
-        <v>1</v>
-      </c>
-      <c r="N64" s="58"/>
+      <c r="L64" s="21"/>
+      <c r="M64" s="10">
+        <v>1</v>
+      </c>
+      <c r="N64" s="3"/>
       <c r="O64" s="3"/>
-      <c r="P64" s="11"/>
-      <c r="Q64" s="12"/>
-      <c r="R64" s="26" t="s">
+      <c r="P64" s="32"/>
+      <c r="Q64" s="33"/>
+      <c r="R64" s="20" t="s">
         <v>17</v>
       </c>
-      <c r="S64" s="27"/>
-      <c r="T64" s="51"/>
+      <c r="S64" s="21"/>
+      <c r="T64" s="10"/>
       <c r="U64" s="3"/>
     </row>
     <row r="65" spans="2:21" x14ac:dyDescent="0.3">
-      <c r="B65" s="11"/>
-      <c r="C65" s="12"/>
-      <c r="D65" s="26" t="s">
+      <c r="B65" s="32"/>
+      <c r="C65" s="33"/>
+      <c r="D65" s="20" t="s">
         <v>8</v>
       </c>
-      <c r="E65" s="27"/>
-      <c r="F65" s="51"/>
-      <c r="G65" s="58"/>
+      <c r="E65" s="21"/>
+      <c r="F65" s="10"/>
+      <c r="G65" s="3"/>
       <c r="H65" s="3"/>
-      <c r="I65" s="11"/>
-      <c r="J65" s="12"/>
-      <c r="K65" s="26" t="s">
+      <c r="I65" s="32"/>
+      <c r="J65" s="33"/>
+      <c r="K65" s="20" t="s">
         <v>6</v>
       </c>
-      <c r="L65" s="27"/>
-      <c r="M65" s="51">
-        <v>1</v>
-      </c>
-      <c r="N65" s="58"/>
+      <c r="L65" s="21"/>
+      <c r="M65" s="10">
+        <v>1</v>
+      </c>
+      <c r="N65" s="3"/>
       <c r="O65" s="3"/>
-      <c r="P65" s="11"/>
-      <c r="Q65" s="12"/>
-      <c r="R65" s="26" t="s">
+      <c r="P65" s="32"/>
+      <c r="Q65" s="33"/>
+      <c r="R65" s="20" t="s">
         <v>8</v>
       </c>
-      <c r="S65" s="27"/>
-      <c r="T65" s="51"/>
+      <c r="S65" s="21"/>
+      <c r="T65" s="10"/>
       <c r="U65" s="3"/>
     </row>
     <row r="66" spans="2:21" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B66" s="13"/>
-      <c r="C66" s="14"/>
-      <c r="D66" s="17" t="s">
+      <c r="B66" s="34"/>
+      <c r="C66" s="35"/>
+      <c r="D66" s="39" t="s">
         <v>41</v>
       </c>
-      <c r="E66" s="18"/>
-      <c r="F66" s="52">
+      <c r="E66" s="40"/>
+      <c r="F66" s="11">
         <f>3-1</f>
         <v>2</v>
       </c>
-      <c r="G66" s="58"/>
+      <c r="G66" s="3"/>
       <c r="H66" s="3"/>
-      <c r="I66" s="13"/>
-      <c r="J66" s="14"/>
-      <c r="K66" s="17" t="s">
+      <c r="I66" s="34"/>
+      <c r="J66" s="35"/>
+      <c r="K66" s="39" t="s">
         <v>63</v>
       </c>
-      <c r="L66" s="18"/>
-      <c r="M66" s="52">
+      <c r="L66" s="40"/>
+      <c r="M66" s="11">
         <f>3-2</f>
         <v>1</v>
       </c>
-      <c r="N66" s="58"/>
+      <c r="N66" s="3"/>
       <c r="O66" s="3"/>
-      <c r="P66" s="13"/>
-      <c r="Q66" s="14"/>
-      <c r="R66" s="56" t="s">
+      <c r="P66" s="34"/>
+      <c r="Q66" s="35"/>
+      <c r="R66" s="28" t="s">
         <v>6</v>
       </c>
-      <c r="S66" s="57"/>
-      <c r="T66" s="52">
+      <c r="S66" s="29"/>
+      <c r="T66" s="11">
         <v>1</v>
       </c>
       <c r="U66" s="3"/>
@@ -3048,7 +3133,158 @@
       <c r="H77" s="1"/>
     </row>
   </sheetData>
-  <mergeCells count="172">
+  <mergeCells count="174">
+    <mergeCell ref="C2:D2"/>
+    <mergeCell ref="E2:Q2"/>
+    <mergeCell ref="I16:J23"/>
+    <mergeCell ref="R21:S21"/>
+    <mergeCell ref="R22:S22"/>
+    <mergeCell ref="R23:S23"/>
+    <mergeCell ref="P16:Q23"/>
+    <mergeCell ref="R13:S13"/>
+    <mergeCell ref="P5:Q13"/>
+    <mergeCell ref="B16:C22"/>
+    <mergeCell ref="D20:E20"/>
+    <mergeCell ref="D21:E21"/>
+    <mergeCell ref="D22:E22"/>
+    <mergeCell ref="K21:L21"/>
+    <mergeCell ref="K22:L22"/>
+    <mergeCell ref="K12:L12"/>
+    <mergeCell ref="I5:J12"/>
+    <mergeCell ref="R12:S12"/>
+    <mergeCell ref="R10:S10"/>
+    <mergeCell ref="R11:S11"/>
+    <mergeCell ref="K10:L10"/>
+    <mergeCell ref="K11:L11"/>
+    <mergeCell ref="R16:S16"/>
+    <mergeCell ref="R17:S17"/>
+    <mergeCell ref="D64:E64"/>
+    <mergeCell ref="D65:E65"/>
+    <mergeCell ref="B60:C66"/>
+    <mergeCell ref="K65:L65"/>
+    <mergeCell ref="K66:L66"/>
+    <mergeCell ref="I60:J66"/>
+    <mergeCell ref="R55:S55"/>
+    <mergeCell ref="K56:L56"/>
+    <mergeCell ref="P63:Q66"/>
+    <mergeCell ref="D63:E63"/>
+    <mergeCell ref="K63:L63"/>
+    <mergeCell ref="D66:E66"/>
+    <mergeCell ref="K64:L64"/>
+    <mergeCell ref="R60:S60"/>
+    <mergeCell ref="R58:S58"/>
+    <mergeCell ref="R64:S64"/>
+    <mergeCell ref="R65:S65"/>
+    <mergeCell ref="R57:S57"/>
+    <mergeCell ref="R63:S63"/>
+    <mergeCell ref="R59:S59"/>
+    <mergeCell ref="R66:S66"/>
+    <mergeCell ref="D62:E62"/>
+    <mergeCell ref="K62:L62"/>
+    <mergeCell ref="D60:E60"/>
+    <mergeCell ref="K60:L60"/>
+    <mergeCell ref="K51:L51"/>
+    <mergeCell ref="D61:E61"/>
+    <mergeCell ref="K61:L61"/>
+    <mergeCell ref="K52:L52"/>
+    <mergeCell ref="R39:S39"/>
+    <mergeCell ref="R41:S41"/>
+    <mergeCell ref="R43:S43"/>
+    <mergeCell ref="R42:S42"/>
+    <mergeCell ref="P36:Q43"/>
+    <mergeCell ref="K55:L55"/>
+    <mergeCell ref="I50:J57"/>
+    <mergeCell ref="P57:Q60"/>
+    <mergeCell ref="D45:E45"/>
+    <mergeCell ref="D47:E47"/>
+    <mergeCell ref="K57:L57"/>
+    <mergeCell ref="K53:L53"/>
+    <mergeCell ref="K54:L54"/>
+    <mergeCell ref="R48:S48"/>
+    <mergeCell ref="K48:L48"/>
+    <mergeCell ref="D54:E54"/>
+    <mergeCell ref="R49:S49"/>
+    <mergeCell ref="R52:S52"/>
+    <mergeCell ref="K44:L44"/>
+    <mergeCell ref="D51:E51"/>
+    <mergeCell ref="R46:S46"/>
+    <mergeCell ref="R47:S47"/>
+    <mergeCell ref="K47:L47"/>
+    <mergeCell ref="K45:L45"/>
+    <mergeCell ref="K43:L43"/>
+    <mergeCell ref="D50:E50"/>
+    <mergeCell ref="K46:L46"/>
+    <mergeCell ref="I43:J48"/>
+    <mergeCell ref="R50:S50"/>
+    <mergeCell ref="R51:S51"/>
+    <mergeCell ref="R45:S45"/>
+    <mergeCell ref="D43:E43"/>
+    <mergeCell ref="D44:E44"/>
+    <mergeCell ref="D46:E46"/>
+    <mergeCell ref="P45:Q55"/>
+    <mergeCell ref="K50:L50"/>
+    <mergeCell ref="R53:S53"/>
+    <mergeCell ref="R54:S54"/>
+    <mergeCell ref="R34:S34"/>
+    <mergeCell ref="D39:E39"/>
+    <mergeCell ref="D37:E37"/>
+    <mergeCell ref="P30:Q34"/>
+    <mergeCell ref="R30:S30"/>
+    <mergeCell ref="D36:E36"/>
+    <mergeCell ref="R33:S33"/>
+    <mergeCell ref="D40:E40"/>
+    <mergeCell ref="R32:S32"/>
+    <mergeCell ref="K32:L32"/>
+    <mergeCell ref="K33:L33"/>
+    <mergeCell ref="R36:S36"/>
+    <mergeCell ref="R37:S37"/>
+    <mergeCell ref="R38:S38"/>
+    <mergeCell ref="K36:L36"/>
+    <mergeCell ref="K37:L37"/>
+    <mergeCell ref="K38:L38"/>
+    <mergeCell ref="K39:L39"/>
+    <mergeCell ref="I36:J39"/>
+    <mergeCell ref="R40:S40"/>
+    <mergeCell ref="R29:S29"/>
+    <mergeCell ref="K31:L31"/>
+    <mergeCell ref="I31:J33"/>
+    <mergeCell ref="K27:L27"/>
+    <mergeCell ref="K28:L28"/>
+    <mergeCell ref="K29:L29"/>
+    <mergeCell ref="K26:L26"/>
+    <mergeCell ref="D27:E27"/>
+    <mergeCell ref="D28:E28"/>
+    <mergeCell ref="D29:E29"/>
+    <mergeCell ref="D30:E30"/>
+    <mergeCell ref="D26:E26"/>
+    <mergeCell ref="R31:S31"/>
+    <mergeCell ref="D31:E31"/>
+    <mergeCell ref="D32:E32"/>
+    <mergeCell ref="D33:E33"/>
+    <mergeCell ref="I26:J28"/>
+    <mergeCell ref="R20:S20"/>
+    <mergeCell ref="K16:L16"/>
+    <mergeCell ref="K17:L17"/>
+    <mergeCell ref="K18:L18"/>
+    <mergeCell ref="K19:L19"/>
+    <mergeCell ref="K20:L20"/>
+    <mergeCell ref="P26:Q28"/>
+    <mergeCell ref="R26:S26"/>
+    <mergeCell ref="R27:S27"/>
+    <mergeCell ref="R28:S28"/>
+    <mergeCell ref="K23:L23"/>
+    <mergeCell ref="R18:S18"/>
+    <mergeCell ref="R19:S19"/>
+    <mergeCell ref="R5:S5"/>
+    <mergeCell ref="R6:S6"/>
+    <mergeCell ref="R7:S7"/>
+    <mergeCell ref="R8:S8"/>
+    <mergeCell ref="R9:S9"/>
+    <mergeCell ref="K5:L5"/>
+    <mergeCell ref="K6:L6"/>
+    <mergeCell ref="K7:L7"/>
+    <mergeCell ref="K8:L8"/>
+    <mergeCell ref="K9:L9"/>
     <mergeCell ref="B4:C4"/>
     <mergeCell ref="D4:E4"/>
     <mergeCell ref="D5:E5"/>
@@ -3071,156 +3307,7 @@
     <mergeCell ref="D53:E53"/>
     <mergeCell ref="D56:E56"/>
     <mergeCell ref="B26:C33"/>
-    <mergeCell ref="R5:S5"/>
-    <mergeCell ref="R6:S6"/>
-    <mergeCell ref="R7:S7"/>
-    <mergeCell ref="R8:S8"/>
-    <mergeCell ref="R9:S9"/>
-    <mergeCell ref="K5:L5"/>
-    <mergeCell ref="K6:L6"/>
-    <mergeCell ref="K7:L7"/>
-    <mergeCell ref="K8:L8"/>
-    <mergeCell ref="K9:L9"/>
-    <mergeCell ref="R20:S20"/>
-    <mergeCell ref="K16:L16"/>
-    <mergeCell ref="K17:L17"/>
-    <mergeCell ref="K18:L18"/>
-    <mergeCell ref="K19:L19"/>
-    <mergeCell ref="K20:L20"/>
-    <mergeCell ref="P26:Q28"/>
-    <mergeCell ref="R26:S26"/>
-    <mergeCell ref="R27:S27"/>
-    <mergeCell ref="R28:S28"/>
-    <mergeCell ref="K23:L23"/>
-    <mergeCell ref="R29:S29"/>
-    <mergeCell ref="K31:L31"/>
-    <mergeCell ref="I31:J33"/>
-    <mergeCell ref="K27:L27"/>
-    <mergeCell ref="K28:L28"/>
-    <mergeCell ref="K29:L29"/>
-    <mergeCell ref="K26:L26"/>
-    <mergeCell ref="D27:E27"/>
-    <mergeCell ref="D28:E28"/>
-    <mergeCell ref="D29:E29"/>
-    <mergeCell ref="D30:E30"/>
-    <mergeCell ref="D26:E26"/>
-    <mergeCell ref="R31:S31"/>
-    <mergeCell ref="D31:E31"/>
-    <mergeCell ref="D32:E32"/>
-    <mergeCell ref="D33:E33"/>
-    <mergeCell ref="I26:J28"/>
-    <mergeCell ref="R34:S34"/>
-    <mergeCell ref="D39:E39"/>
-    <mergeCell ref="D37:E37"/>
-    <mergeCell ref="P30:Q34"/>
-    <mergeCell ref="R30:S30"/>
-    <mergeCell ref="D36:E36"/>
-    <mergeCell ref="R33:S33"/>
-    <mergeCell ref="D40:E40"/>
-    <mergeCell ref="R32:S32"/>
-    <mergeCell ref="K32:L32"/>
-    <mergeCell ref="K33:L33"/>
-    <mergeCell ref="R36:S36"/>
-    <mergeCell ref="R37:S37"/>
-    <mergeCell ref="R38:S38"/>
     <mergeCell ref="B36:C40"/>
-    <mergeCell ref="K44:L44"/>
-    <mergeCell ref="D51:E51"/>
-    <mergeCell ref="R46:S46"/>
-    <mergeCell ref="R47:S47"/>
-    <mergeCell ref="K47:L47"/>
-    <mergeCell ref="K45:L45"/>
-    <mergeCell ref="K43:L43"/>
-    <mergeCell ref="D50:E50"/>
-    <mergeCell ref="K46:L46"/>
-    <mergeCell ref="I43:J48"/>
-    <mergeCell ref="R50:S50"/>
-    <mergeCell ref="R51:S51"/>
-    <mergeCell ref="R45:S45"/>
-    <mergeCell ref="K36:L36"/>
-    <mergeCell ref="K37:L37"/>
-    <mergeCell ref="K38:L38"/>
-    <mergeCell ref="K39:L39"/>
-    <mergeCell ref="I36:J39"/>
-    <mergeCell ref="R40:S40"/>
-    <mergeCell ref="D43:E43"/>
-    <mergeCell ref="D44:E44"/>
-    <mergeCell ref="D46:E46"/>
-    <mergeCell ref="P45:Q55"/>
-    <mergeCell ref="K50:L50"/>
-    <mergeCell ref="D60:E60"/>
-    <mergeCell ref="K60:L60"/>
-    <mergeCell ref="K51:L51"/>
-    <mergeCell ref="D61:E61"/>
-    <mergeCell ref="K61:L61"/>
-    <mergeCell ref="K52:L52"/>
-    <mergeCell ref="R39:S39"/>
-    <mergeCell ref="R41:S41"/>
-    <mergeCell ref="R43:S43"/>
-    <mergeCell ref="R42:S42"/>
-    <mergeCell ref="P36:Q43"/>
-    <mergeCell ref="K55:L55"/>
-    <mergeCell ref="I50:J57"/>
-    <mergeCell ref="P57:Q60"/>
-    <mergeCell ref="D45:E45"/>
-    <mergeCell ref="D47:E47"/>
-    <mergeCell ref="K57:L57"/>
-    <mergeCell ref="D64:E64"/>
-    <mergeCell ref="D65:E65"/>
-    <mergeCell ref="B60:C66"/>
-    <mergeCell ref="K65:L65"/>
-    <mergeCell ref="K66:L66"/>
-    <mergeCell ref="I60:J66"/>
-    <mergeCell ref="R55:S55"/>
-    <mergeCell ref="K56:L56"/>
-    <mergeCell ref="P63:Q66"/>
-    <mergeCell ref="K53:L53"/>
-    <mergeCell ref="D63:E63"/>
-    <mergeCell ref="K63:L63"/>
-    <mergeCell ref="K54:L54"/>
-    <mergeCell ref="D66:E66"/>
-    <mergeCell ref="K64:L64"/>
-    <mergeCell ref="R48:S48"/>
-    <mergeCell ref="K48:L48"/>
-    <mergeCell ref="D54:E54"/>
-    <mergeCell ref="R49:S49"/>
-    <mergeCell ref="R52:S52"/>
-    <mergeCell ref="R53:S53"/>
-    <mergeCell ref="R54:S54"/>
-    <mergeCell ref="R60:S60"/>
-    <mergeCell ref="R58:S58"/>
-    <mergeCell ref="R64:S64"/>
-    <mergeCell ref="R65:S65"/>
-    <mergeCell ref="R57:S57"/>
-    <mergeCell ref="R63:S63"/>
-    <mergeCell ref="R59:S59"/>
-    <mergeCell ref="R66:S66"/>
-    <mergeCell ref="D62:E62"/>
-    <mergeCell ref="K62:L62"/>
-    <mergeCell ref="I16:J23"/>
-    <mergeCell ref="R21:S21"/>
-    <mergeCell ref="R22:S22"/>
-    <mergeCell ref="R23:S23"/>
-    <mergeCell ref="P16:Q23"/>
-    <mergeCell ref="R13:S13"/>
-    <mergeCell ref="P5:Q13"/>
-    <mergeCell ref="B16:C22"/>
-    <mergeCell ref="D20:E20"/>
-    <mergeCell ref="D21:E21"/>
-    <mergeCell ref="D22:E22"/>
-    <mergeCell ref="K21:L21"/>
-    <mergeCell ref="K22:L22"/>
-    <mergeCell ref="K12:L12"/>
-    <mergeCell ref="I5:J12"/>
-    <mergeCell ref="R12:S12"/>
-    <mergeCell ref="R10:S10"/>
-    <mergeCell ref="R11:S11"/>
-    <mergeCell ref="K10:L10"/>
-    <mergeCell ref="K11:L11"/>
-    <mergeCell ref="R16:S16"/>
-    <mergeCell ref="R17:S17"/>
-    <mergeCell ref="R18:S18"/>
-    <mergeCell ref="R19:S19"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -3232,133 +3319,133 @@
   <dimension ref="B2:M45"/>
   <sheetViews>
     <sheetView topLeftCell="A12" workbookViewId="0">
-      <selection activeCell="M25" sqref="M25"/>
+      <selection activeCell="K20" sqref="K20:L20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="2" spans="2:13" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="3" spans="2:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="46" t="s">
+      <c r="B3" s="66" t="s">
         <v>3</v>
       </c>
-      <c r="C3" s="47"/>
+      <c r="C3" s="67"/>
       <c r="D3" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="F3" s="44" t="s">
+      <c r="F3" s="64" t="s">
         <v>19</v>
       </c>
-      <c r="G3" s="45"/>
-      <c r="I3" s="9" t="s">
+      <c r="G3" s="65"/>
+      <c r="I3" s="15" t="s">
         <v>0</v>
       </c>
-      <c r="J3" s="10"/>
-      <c r="K3" s="42" t="s">
-        <v>1</v>
-      </c>
-      <c r="L3" s="43"/>
+      <c r="J3" s="16"/>
+      <c r="K3" s="73" t="s">
+        <v>1</v>
+      </c>
+      <c r="L3" s="74"/>
       <c r="M3" s="7" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="4" spans="2:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B4" s="24" t="s">
+      <c r="B4" s="62" t="s">
         <v>4</v>
       </c>
-      <c r="C4" s="25"/>
+      <c r="C4" s="63"/>
       <c r="D4" s="8">
         <v>1</v>
       </c>
-      <c r="I4" s="33" t="s">
+      <c r="I4" s="56" t="s">
         <v>40</v>
       </c>
-      <c r="J4" s="34"/>
-      <c r="K4" s="15" t="s">
+      <c r="J4" s="70"/>
+      <c r="K4" s="52" t="s">
         <v>5</v>
       </c>
-      <c r="L4" s="16"/>
-      <c r="M4" s="50">
+      <c r="L4" s="53"/>
+      <c r="M4" s="9">
         <v>1</v>
       </c>
     </row>
     <row r="5" spans="2:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B5" s="15" t="s">
+      <c r="B5" s="52" t="s">
         <v>5</v>
       </c>
-      <c r="C5" s="16"/>
+      <c r="C5" s="53"/>
       <c r="D5" s="5">
         <v>1</v>
       </c>
-      <c r="F5" s="48" t="s">
+      <c r="F5" s="68" t="s">
         <v>51</v>
       </c>
-      <c r="G5" s="49"/>
-      <c r="I5" s="35"/>
-      <c r="J5" s="36"/>
-      <c r="K5" s="15" t="s">
+      <c r="G5" s="69"/>
+      <c r="I5" s="58"/>
+      <c r="J5" s="71"/>
+      <c r="K5" s="52" t="s">
         <v>6</v>
       </c>
-      <c r="L5" s="16"/>
-      <c r="M5" s="51">
+      <c r="L5" s="53"/>
+      <c r="M5" s="10">
         <v>1</v>
       </c>
     </row>
     <row r="6" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B6" s="15" t="s">
+      <c r="B6" s="52" t="s">
         <v>47</v>
       </c>
-      <c r="C6" s="16"/>
+      <c r="C6" s="53"/>
       <c r="D6" s="5">
         <v>1</v>
       </c>
-      <c r="I6" s="35"/>
-      <c r="J6" s="36"/>
-      <c r="K6" s="15" t="s">
+      <c r="I6" s="58"/>
+      <c r="J6" s="71"/>
+      <c r="K6" s="52" t="s">
         <v>7</v>
       </c>
-      <c r="L6" s="16"/>
-      <c r="M6" s="51">
+      <c r="L6" s="53"/>
+      <c r="M6" s="10">
         <v>1</v>
       </c>
     </row>
     <row r="7" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B7" s="15" t="s">
+      <c r="B7" s="52" t="s">
         <v>6</v>
       </c>
-      <c r="C7" s="16"/>
+      <c r="C7" s="53"/>
       <c r="D7" s="5">
         <v>1</v>
       </c>
-      <c r="I7" s="35"/>
-      <c r="J7" s="36"/>
-      <c r="K7" s="15" t="s">
+      <c r="I7" s="58"/>
+      <c r="J7" s="71"/>
+      <c r="K7" s="52" t="s">
         <v>8</v>
       </c>
-      <c r="L7" s="16"/>
-      <c r="M7" s="51"/>
+      <c r="L7" s="53"/>
+      <c r="M7" s="10"/>
     </row>
     <row r="8" spans="2:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B8" s="15" t="s">
+      <c r="B8" s="52" t="s">
         <v>7</v>
       </c>
-      <c r="C8" s="16"/>
+      <c r="C8" s="53"/>
       <c r="D8" s="5">
         <v>1</v>
       </c>
-      <c r="I8" s="37"/>
-      <c r="J8" s="38"/>
-      <c r="K8" s="22" t="s">
+      <c r="I8" s="60"/>
+      <c r="J8" s="72"/>
+      <c r="K8" s="54" t="s">
         <v>13</v>
       </c>
-      <c r="L8" s="23"/>
-      <c r="M8" s="52"/>
+      <c r="L8" s="55"/>
+      <c r="M8" s="11"/>
     </row>
     <row r="9" spans="2:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B9" s="15" t="s">
+      <c r="B9" s="52" t="s">
         <v>10</v>
       </c>
-      <c r="C9" s="16"/>
+      <c r="C9" s="53"/>
       <c r="D9" s="5">
         <v>1</v>
       </c>
@@ -3367,368 +3454,368 @@
       </c>
     </row>
     <row r="10" spans="2:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B10" s="15" t="s">
+      <c r="B10" s="52" t="s">
         <v>65</v>
       </c>
-      <c r="C10" s="16"/>
+      <c r="C10" s="53"/>
       <c r="D10" s="5">
         <v>1</v>
       </c>
-      <c r="M10" s="53"/>
+      <c r="M10" s="12"/>
     </row>
     <row r="11" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B11" s="15" t="s">
+      <c r="B11" s="52" t="s">
         <v>14</v>
       </c>
-      <c r="C11" s="16"/>
+      <c r="C11" s="53"/>
       <c r="D11" s="5">
         <v>1</v>
       </c>
-      <c r="I11" s="33" t="s">
+      <c r="I11" s="56" t="s">
         <v>44</v>
       </c>
-      <c r="J11" s="34"/>
-      <c r="K11" s="24" t="s">
+      <c r="J11" s="70"/>
+      <c r="K11" s="62" t="s">
         <v>4</v>
       </c>
-      <c r="L11" s="25"/>
-      <c r="M11" s="50">
+      <c r="L11" s="63"/>
+      <c r="M11" s="9">
         <v>1</v>
       </c>
     </row>
     <row r="12" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B12" s="15" t="s">
+      <c r="B12" s="52" t="s">
         <v>49</v>
       </c>
-      <c r="C12" s="16"/>
+      <c r="C12" s="53"/>
       <c r="D12" s="5">
         <v>1</v>
       </c>
-      <c r="I12" s="35"/>
-      <c r="J12" s="36"/>
-      <c r="K12" s="15" t="s">
+      <c r="I12" s="58"/>
+      <c r="J12" s="71"/>
+      <c r="K12" s="52" t="s">
         <v>15</v>
       </c>
-      <c r="L12" s="16"/>
-      <c r="M12" s="51"/>
+      <c r="L12" s="53"/>
+      <c r="M12" s="10"/>
     </row>
     <row r="13" spans="2:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B13" s="15" t="s">
+      <c r="B13" s="52" t="s">
         <v>50</v>
       </c>
-      <c r="C13" s="16"/>
+      <c r="C13" s="53"/>
       <c r="D13" s="5">
         <v>1</v>
       </c>
-      <c r="I13" s="37"/>
-      <c r="J13" s="38"/>
-      <c r="K13" s="22" t="s">
+      <c r="I13" s="60"/>
+      <c r="J13" s="72"/>
+      <c r="K13" s="54" t="s">
         <v>10</v>
       </c>
-      <c r="L13" s="23"/>
-      <c r="M13" s="52">
+      <c r="L13" s="55"/>
+      <c r="M13" s="11">
         <v>1</v>
       </c>
     </row>
     <row r="14" spans="2:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B14" s="15" t="s">
+      <c r="B14" s="52" t="s">
         <v>59</v>
       </c>
-      <c r="C14" s="16"/>
+      <c r="C14" s="53"/>
       <c r="D14" s="5">
         <v>1</v>
       </c>
-      <c r="M14" s="55">
+      <c r="M14" s="14">
         <v>2</v>
       </c>
     </row>
     <row r="15" spans="2:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B15" s="15" t="s">
+      <c r="B15" s="52" t="s">
         <v>11</v>
       </c>
-      <c r="C15" s="16"/>
+      <c r="C15" s="53"/>
       <c r="D15" s="5"/>
-      <c r="M15" s="53"/>
+      <c r="M15" s="12"/>
     </row>
     <row r="16" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B16" s="15" t="s">
+      <c r="B16" s="52" t="s">
         <v>48</v>
       </c>
-      <c r="C16" s="16"/>
+      <c r="C16" s="53"/>
       <c r="D16" s="5"/>
-      <c r="I16" s="33" t="s">
+      <c r="I16" s="56" t="s">
         <v>52</v>
       </c>
-      <c r="J16" s="39"/>
-      <c r="K16" s="24" t="s">
+      <c r="J16" s="57"/>
+      <c r="K16" s="62" t="s">
         <v>5</v>
       </c>
-      <c r="L16" s="25"/>
-      <c r="M16" s="50">
+      <c r="L16" s="63"/>
+      <c r="M16" s="9">
         <v>1</v>
       </c>
     </row>
     <row r="17" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B17" s="15" t="s">
+      <c r="B17" s="52" t="s">
         <v>8</v>
       </c>
-      <c r="C17" s="16"/>
+      <c r="C17" s="53"/>
       <c r="D17" s="5"/>
-      <c r="I17" s="35"/>
-      <c r="J17" s="40"/>
-      <c r="K17" s="15" t="s">
+      <c r="I17" s="58"/>
+      <c r="J17" s="59"/>
+      <c r="K17" s="52" t="s">
         <v>6</v>
       </c>
-      <c r="L17" s="16"/>
-      <c r="M17" s="51">
+      <c r="L17" s="53"/>
+      <c r="M17" s="10">
         <v>1</v>
       </c>
     </row>
     <row r="18" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B18" s="15" t="s">
+      <c r="B18" s="52" t="s">
         <v>13</v>
       </c>
-      <c r="C18" s="16"/>
+      <c r="C18" s="53"/>
       <c r="D18" s="5"/>
-      <c r="I18" s="35"/>
-      <c r="J18" s="40"/>
-      <c r="K18" s="15" t="s">
+      <c r="I18" s="58"/>
+      <c r="J18" s="59"/>
+      <c r="K18" s="52" t="s">
         <v>7</v>
       </c>
-      <c r="L18" s="16"/>
-      <c r="M18" s="51">
+      <c r="L18" s="53"/>
+      <c r="M18" s="10">
         <v>1</v>
       </c>
     </row>
     <row r="19" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B19" s="15" t="s">
+      <c r="B19" s="52" t="s">
         <v>61</v>
       </c>
-      <c r="C19" s="16"/>
+      <c r="C19" s="53"/>
       <c r="D19" s="5"/>
-      <c r="I19" s="35"/>
-      <c r="J19" s="40"/>
-      <c r="K19" s="15" t="s">
+      <c r="I19" s="58"/>
+      <c r="J19" s="59"/>
+      <c r="K19" s="52" t="s">
         <v>8</v>
       </c>
-      <c r="L19" s="16"/>
-      <c r="M19" s="51"/>
+      <c r="L19" s="53"/>
+      <c r="M19" s="10"/>
     </row>
     <row r="20" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B20" s="15" t="s">
+      <c r="B20" s="52" t="s">
         <v>15</v>
       </c>
-      <c r="C20" s="16"/>
+      <c r="C20" s="53"/>
       <c r="D20" s="5"/>
-      <c r="I20" s="35"/>
-      <c r="J20" s="40"/>
-      <c r="K20" s="15" t="s">
+      <c r="I20" s="58"/>
+      <c r="J20" s="59"/>
+      <c r="K20" s="52" t="s">
         <v>11</v>
       </c>
-      <c r="L20" s="16"/>
-      <c r="M20" s="51"/>
+      <c r="L20" s="53"/>
+      <c r="M20" s="10"/>
     </row>
     <row r="21" spans="2:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B21" s="15" t="s">
+      <c r="B21" s="52" t="s">
         <v>16</v>
       </c>
-      <c r="C21" s="16"/>
+      <c r="C21" s="53"/>
       <c r="D21" s="5"/>
-      <c r="I21" s="37"/>
-      <c r="J21" s="41"/>
-      <c r="K21" s="22" t="s">
+      <c r="I21" s="60"/>
+      <c r="J21" s="61"/>
+      <c r="K21" s="54" t="s">
         <v>10</v>
       </c>
-      <c r="L21" s="23"/>
-      <c r="M21" s="54">
+      <c r="L21" s="55"/>
+      <c r="M21" s="13">
         <v>1</v>
       </c>
     </row>
     <row r="22" spans="2:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B22" s="15" t="s">
+      <c r="B22" s="52" t="s">
         <v>17</v>
       </c>
-      <c r="C22" s="16"/>
+      <c r="C22" s="53"/>
       <c r="D22" s="5"/>
       <c r="M22" s="4">
         <v>4</v>
       </c>
     </row>
     <row r="23" spans="2:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B23" s="15" t="s">
+      <c r="B23" s="52" t="s">
         <v>42</v>
       </c>
-      <c r="C23" s="16"/>
+      <c r="C23" s="53"/>
       <c r="D23" s="5"/>
-      <c r="M23" s="53"/>
+      <c r="M23" s="12"/>
     </row>
     <row r="24" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B24" s="15" t="s">
+      <c r="B24" s="52" t="s">
         <v>43</v>
       </c>
-      <c r="C24" s="16"/>
+      <c r="C24" s="53"/>
       <c r="D24" s="5"/>
-      <c r="I24" s="33" t="s">
+      <c r="I24" s="56" t="s">
         <v>56</v>
       </c>
-      <c r="J24" s="39"/>
-      <c r="K24" s="24" t="s">
+      <c r="J24" s="57"/>
+      <c r="K24" s="62" t="s">
         <v>54</v>
       </c>
-      <c r="L24" s="25"/>
-      <c r="M24" s="50"/>
+      <c r="L24" s="63"/>
+      <c r="M24" s="9"/>
     </row>
     <row r="25" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B25" s="15" t="s">
+      <c r="B25" s="52" t="s">
         <v>45</v>
       </c>
-      <c r="C25" s="16"/>
+      <c r="C25" s="53"/>
       <c r="D25" s="5"/>
-      <c r="I25" s="35"/>
-      <c r="J25" s="40"/>
-      <c r="K25" s="15" t="s">
+      <c r="I25" s="58"/>
+      <c r="J25" s="59"/>
+      <c r="K25" s="52" t="s">
         <v>6</v>
       </c>
-      <c r="L25" s="16"/>
-      <c r="M25" s="51">
+      <c r="L25" s="53"/>
+      <c r="M25" s="10">
         <v>1</v>
       </c>
     </row>
     <row r="26" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B26" s="15" t="s">
+      <c r="B26" s="52" t="s">
         <v>46</v>
       </c>
-      <c r="C26" s="16"/>
+      <c r="C26" s="53"/>
       <c r="D26" s="5"/>
-      <c r="I26" s="35"/>
-      <c r="J26" s="40"/>
-      <c r="K26" s="15" t="s">
+      <c r="I26" s="58"/>
+      <c r="J26" s="59"/>
+      <c r="K26" s="52" t="s">
         <v>7</v>
       </c>
-      <c r="L26" s="16"/>
-      <c r="M26" s="51">
+      <c r="L26" s="53"/>
+      <c r="M26" s="10">
         <v>1</v>
       </c>
     </row>
     <row r="27" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B27" s="15" t="s">
+      <c r="B27" s="52" t="s">
         <v>62</v>
       </c>
-      <c r="C27" s="16"/>
+      <c r="C27" s="53"/>
       <c r="D27" s="5"/>
-      <c r="I27" s="35"/>
-      <c r="J27" s="40"/>
-      <c r="K27" s="15" t="s">
+      <c r="I27" s="58"/>
+      <c r="J27" s="59"/>
+      <c r="K27" s="52" t="s">
         <v>8</v>
       </c>
-      <c r="L27" s="16"/>
-      <c r="M27" s="51"/>
+      <c r="L27" s="53"/>
+      <c r="M27" s="10"/>
     </row>
     <row r="28" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B28" s="15" t="s">
+      <c r="B28" s="52" t="s">
         <v>9</v>
       </c>
-      <c r="C28" s="16"/>
+      <c r="C28" s="53"/>
       <c r="D28" s="5"/>
-      <c r="I28" s="35"/>
-      <c r="J28" s="40"/>
-      <c r="K28" s="15" t="s">
+      <c r="I28" s="58"/>
+      <c r="J28" s="59"/>
+      <c r="K28" s="52" t="s">
         <v>55</v>
       </c>
-      <c r="L28" s="16"/>
-      <c r="M28" s="51"/>
+      <c r="L28" s="53"/>
+      <c r="M28" s="10"/>
     </row>
     <row r="29" spans="2:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B29" s="15" t="s">
+      <c r="B29" s="52" t="s">
         <v>54</v>
       </c>
-      <c r="C29" s="16"/>
+      <c r="C29" s="53"/>
       <c r="D29" s="5"/>
-      <c r="I29" s="37"/>
-      <c r="J29" s="41"/>
-      <c r="K29" s="22" t="s">
+      <c r="I29" s="60"/>
+      <c r="J29" s="61"/>
+      <c r="K29" s="54" t="s">
         <v>10</v>
       </c>
-      <c r="L29" s="23"/>
-      <c r="M29" s="54">
+      <c r="L29" s="55"/>
+      <c r="M29" s="13">
         <v>1</v>
       </c>
     </row>
     <row r="30" spans="2:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B30" s="15" t="s">
+      <c r="B30" s="52" t="s">
         <v>55</v>
       </c>
-      <c r="C30" s="16"/>
+      <c r="C30" s="53"/>
       <c r="D30" s="5"/>
       <c r="M30" s="4">
         <v>3</v>
       </c>
     </row>
     <row r="31" spans="2:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B31" s="22" t="s">
+      <c r="B31" s="54" t="s">
         <v>60</v>
       </c>
-      <c r="C31" s="23"/>
+      <c r="C31" s="55"/>
       <c r="D31" s="6"/>
-      <c r="M31" s="53"/>
+      <c r="M31" s="12"/>
     </row>
     <row r="32" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="I32" s="33" t="s">
+      <c r="I32" s="56" t="s">
         <v>58</v>
       </c>
-      <c r="J32" s="39"/>
-      <c r="K32" s="24" t="s">
+      <c r="J32" s="57"/>
+      <c r="K32" s="62" t="s">
         <v>8</v>
       </c>
-      <c r="L32" s="25"/>
-      <c r="M32" s="50"/>
+      <c r="L32" s="63"/>
+      <c r="M32" s="9"/>
     </row>
     <row r="33" spans="9:13" x14ac:dyDescent="0.3">
-      <c r="I33" s="35"/>
-      <c r="J33" s="40"/>
-      <c r="K33" s="15" t="s">
+      <c r="I33" s="58"/>
+      <c r="J33" s="59"/>
+      <c r="K33" s="52" t="s">
         <v>4</v>
       </c>
-      <c r="L33" s="16"/>
-      <c r="M33" s="51">
+      <c r="L33" s="53"/>
+      <c r="M33" s="10">
         <v>1</v>
       </c>
     </row>
     <row r="34" spans="9:13" x14ac:dyDescent="0.3">
-      <c r="I34" s="35"/>
-      <c r="J34" s="40"/>
-      <c r="K34" s="15" t="s">
+      <c r="I34" s="58"/>
+      <c r="J34" s="59"/>
+      <c r="K34" s="52" t="s">
         <v>9</v>
       </c>
-      <c r="L34" s="16"/>
-      <c r="M34" s="51"/>
+      <c r="L34" s="53"/>
+      <c r="M34" s="10"/>
     </row>
     <row r="35" spans="9:13" x14ac:dyDescent="0.3">
-      <c r="I35" s="35"/>
-      <c r="J35" s="40"/>
-      <c r="K35" s="15" t="s">
+      <c r="I35" s="58"/>
+      <c r="J35" s="59"/>
+      <c r="K35" s="52" t="s">
         <v>54</v>
       </c>
-      <c r="L35" s="16"/>
-      <c r="M35" s="51"/>
+      <c r="L35" s="53"/>
+      <c r="M35" s="10"/>
     </row>
     <row r="36" spans="9:13" x14ac:dyDescent="0.3">
-      <c r="I36" s="35"/>
-      <c r="J36" s="40"/>
-      <c r="K36" s="15" t="s">
+      <c r="I36" s="58"/>
+      <c r="J36" s="59"/>
+      <c r="K36" s="52" t="s">
         <v>15</v>
       </c>
-      <c r="L36" s="16"/>
-      <c r="M36" s="51"/>
+      <c r="L36" s="53"/>
+      <c r="M36" s="10"/>
     </row>
     <row r="37" spans="9:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="I37" s="37"/>
-      <c r="J37" s="41"/>
-      <c r="K37" s="22" t="s">
+      <c r="I37" s="60"/>
+      <c r="J37" s="61"/>
+      <c r="K37" s="54" t="s">
         <v>6</v>
       </c>
-      <c r="L37" s="23"/>
-      <c r="M37" s="54">
+      <c r="L37" s="55"/>
+      <c r="M37" s="13">
         <v>1</v>
       </c>
     </row>
@@ -3738,60 +3825,60 @@
       </c>
     </row>
     <row r="39" spans="9:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="M39" s="53"/>
+      <c r="M39" s="12"/>
     </row>
     <row r="40" spans="9:13" x14ac:dyDescent="0.3">
-      <c r="I40" s="33" t="s">
+      <c r="I40" s="56" t="s">
         <v>63</v>
       </c>
-      <c r="J40" s="39"/>
-      <c r="K40" s="24" t="s">
+      <c r="J40" s="57"/>
+      <c r="K40" s="62" t="s">
         <v>8</v>
       </c>
-      <c r="L40" s="25"/>
-      <c r="M40" s="50"/>
+      <c r="L40" s="63"/>
+      <c r="M40" s="9"/>
     </row>
     <row r="41" spans="9:13" x14ac:dyDescent="0.3">
-      <c r="I41" s="35"/>
-      <c r="J41" s="40"/>
-      <c r="K41" s="15" t="s">
+      <c r="I41" s="58"/>
+      <c r="J41" s="59"/>
+      <c r="K41" s="52" t="s">
         <v>4</v>
       </c>
-      <c r="L41" s="16"/>
-      <c r="M41" s="51">
+      <c r="L41" s="53"/>
+      <c r="M41" s="10">
         <v>1</v>
       </c>
     </row>
     <row r="42" spans="9:13" x14ac:dyDescent="0.3">
-      <c r="I42" s="35"/>
-      <c r="J42" s="40"/>
-      <c r="K42" s="15" t="s">
+      <c r="I42" s="58"/>
+      <c r="J42" s="59"/>
+      <c r="K42" s="52" t="s">
         <v>10</v>
       </c>
-      <c r="L42" s="16"/>
-      <c r="M42" s="51">
+      <c r="L42" s="53"/>
+      <c r="M42" s="10">
         <v>1</v>
       </c>
     </row>
     <row r="43" spans="9:13" x14ac:dyDescent="0.3">
-      <c r="I43" s="35"/>
-      <c r="J43" s="40"/>
-      <c r="K43" s="15" t="s">
+      <c r="I43" s="58"/>
+      <c r="J43" s="59"/>
+      <c r="K43" s="52" t="s">
         <v>6</v>
       </c>
-      <c r="L43" s="16"/>
-      <c r="M43" s="51">
+      <c r="L43" s="53"/>
+      <c r="M43" s="10">
         <v>1</v>
       </c>
     </row>
     <row r="44" spans="9:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="I44" s="37"/>
-      <c r="J44" s="41"/>
-      <c r="K44" s="22" t="s">
+      <c r="I44" s="60"/>
+      <c r="J44" s="61"/>
+      <c r="K44" s="54" t="s">
         <v>15</v>
       </c>
-      <c r="L44" s="23"/>
-      <c r="M44" s="52"/>
+      <c r="L44" s="55"/>
+      <c r="M44" s="11"/>
     </row>
     <row r="45" spans="9:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="M45" s="4">
@@ -3800,6 +3887,63 @@
     </row>
   </sheetData>
   <mergeCells count="70">
+    <mergeCell ref="K7:L7"/>
+    <mergeCell ref="K8:L8"/>
+    <mergeCell ref="I4:J8"/>
+    <mergeCell ref="I3:J3"/>
+    <mergeCell ref="K3:L3"/>
+    <mergeCell ref="K4:L4"/>
+    <mergeCell ref="K5:L5"/>
+    <mergeCell ref="K6:L6"/>
+    <mergeCell ref="K21:L21"/>
+    <mergeCell ref="I16:J21"/>
+    <mergeCell ref="K16:L16"/>
+    <mergeCell ref="K17:L17"/>
+    <mergeCell ref="K18:L18"/>
+    <mergeCell ref="K19:L19"/>
+    <mergeCell ref="K20:L20"/>
+    <mergeCell ref="B8:C8"/>
+    <mergeCell ref="B17:C17"/>
+    <mergeCell ref="K11:L11"/>
+    <mergeCell ref="K12:L12"/>
+    <mergeCell ref="K13:L13"/>
+    <mergeCell ref="I11:J13"/>
+    <mergeCell ref="B9:C9"/>
+    <mergeCell ref="B15:C15"/>
+    <mergeCell ref="B16:C16"/>
+    <mergeCell ref="B31:C31"/>
+    <mergeCell ref="B22:C22"/>
+    <mergeCell ref="B23:C23"/>
+    <mergeCell ref="B24:C24"/>
+    <mergeCell ref="B25:C25"/>
+    <mergeCell ref="B30:C30"/>
+    <mergeCell ref="B26:C26"/>
+    <mergeCell ref="B29:C29"/>
+    <mergeCell ref="B28:C28"/>
+    <mergeCell ref="B27:C27"/>
+    <mergeCell ref="B18:C18"/>
+    <mergeCell ref="B10:C10"/>
+    <mergeCell ref="B14:C14"/>
+    <mergeCell ref="B21:C21"/>
+    <mergeCell ref="B11:C11"/>
+    <mergeCell ref="B20:C20"/>
+    <mergeCell ref="B12:C12"/>
+    <mergeCell ref="B13:C13"/>
+    <mergeCell ref="B19:C19"/>
+    <mergeCell ref="F3:G3"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="B5:C5"/>
+    <mergeCell ref="B7:C7"/>
+    <mergeCell ref="F5:G5"/>
+    <mergeCell ref="B6:C6"/>
+    <mergeCell ref="I24:J29"/>
+    <mergeCell ref="K24:L24"/>
+    <mergeCell ref="K25:L25"/>
+    <mergeCell ref="K26:L26"/>
+    <mergeCell ref="K27:L27"/>
+    <mergeCell ref="K28:L28"/>
+    <mergeCell ref="K29:L29"/>
     <mergeCell ref="K42:L42"/>
     <mergeCell ref="K44:L44"/>
     <mergeCell ref="K43:L43"/>
@@ -3813,63 +3957,6 @@
     <mergeCell ref="K37:L37"/>
     <mergeCell ref="K40:L40"/>
     <mergeCell ref="K41:L41"/>
-    <mergeCell ref="I24:J29"/>
-    <mergeCell ref="K24:L24"/>
-    <mergeCell ref="K25:L25"/>
-    <mergeCell ref="K26:L26"/>
-    <mergeCell ref="K27:L27"/>
-    <mergeCell ref="K28:L28"/>
-    <mergeCell ref="K29:L29"/>
-    <mergeCell ref="F3:G3"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="B4:C4"/>
-    <mergeCell ref="B5:C5"/>
-    <mergeCell ref="B7:C7"/>
-    <mergeCell ref="F5:G5"/>
-    <mergeCell ref="B6:C6"/>
-    <mergeCell ref="B28:C28"/>
-    <mergeCell ref="B9:C9"/>
-    <mergeCell ref="B15:C15"/>
-    <mergeCell ref="B16:C16"/>
-    <mergeCell ref="B18:C18"/>
-    <mergeCell ref="B10:C10"/>
-    <mergeCell ref="B31:C31"/>
-    <mergeCell ref="B22:C22"/>
-    <mergeCell ref="B23:C23"/>
-    <mergeCell ref="B24:C24"/>
-    <mergeCell ref="B25:C25"/>
-    <mergeCell ref="B30:C30"/>
-    <mergeCell ref="B14:C14"/>
-    <mergeCell ref="B21:C21"/>
-    <mergeCell ref="B11:C11"/>
-    <mergeCell ref="B20:C20"/>
-    <mergeCell ref="B26:C26"/>
-    <mergeCell ref="B12:C12"/>
-    <mergeCell ref="B13:C13"/>
-    <mergeCell ref="B29:C29"/>
-    <mergeCell ref="K7:L7"/>
-    <mergeCell ref="K8:L8"/>
-    <mergeCell ref="I4:J8"/>
-    <mergeCell ref="B19:C19"/>
-    <mergeCell ref="B27:C27"/>
-    <mergeCell ref="B8:C8"/>
-    <mergeCell ref="B17:C17"/>
-    <mergeCell ref="I3:J3"/>
-    <mergeCell ref="K3:L3"/>
-    <mergeCell ref="K4:L4"/>
-    <mergeCell ref="K5:L5"/>
-    <mergeCell ref="K6:L6"/>
-    <mergeCell ref="K11:L11"/>
-    <mergeCell ref="K12:L12"/>
-    <mergeCell ref="K13:L13"/>
-    <mergeCell ref="I11:J13"/>
-    <mergeCell ref="K21:L21"/>
-    <mergeCell ref="I16:J21"/>
-    <mergeCell ref="K16:L16"/>
-    <mergeCell ref="K17:L17"/>
-    <mergeCell ref="K18:L18"/>
-    <mergeCell ref="K19:L19"/>
-    <mergeCell ref="K20:L20"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>